<commit_message>
Added new unit-tests for curation rewards + some refactorings
</commit_message>
<xml_diff>
--- a/doc/curation-rewards-old-new-algorithm.xlsx
+++ b/doc/curation-rewards-old-new-algorithm.xlsx
@@ -77,7 +77,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="18">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -118,8 +118,50 @@
     </font>
     <font>
       <sz val="10"/>
+      <color rgb="FFCE181E"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFCE181E"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF407927"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF407927"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00508F"/>
+      <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF00508F"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -193,7 +235,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="14">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -226,6 +268,30 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -239,7 +305,7 @@
     <indexedColors>
       <rgbColor rgb="FF000000"/>
       <rgbColor rgb="FFFFFFFF"/>
-      <rgbColor rgb="FFFF0000"/>
+      <rgbColor rgb="FFCE181E"/>
       <rgbColor rgb="FF00FF00"/>
       <rgbColor rgb="FF0000FF"/>
       <rgbColor rgb="FFFFFF00"/>
@@ -285,8 +351,8 @@
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FFB3B3B3"/>
-      <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF00508F"/>
+      <rgbColor rgb="FF407927"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -298,7 +364,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1340,11 +1406,11 @@
           </c:yVal>
           <c:smooth val="1"/>
         </c:ser>
-        <c:axId val="25111096"/>
-        <c:axId val="99901786"/>
+        <c:axId val="56762319"/>
+        <c:axId val="75135029"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="25111096"/>
+        <c:axId val="56762319"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1407,12 +1473,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="99901786"/>
+        <c:crossAx val="75135029"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="99901786"/>
+        <c:axId val="75135029"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1485,7 +1551,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="25111096"/>
+        <c:crossAx val="56762319"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1512,7 +1578,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2557,11 +2623,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="50364798"/>
-        <c:axId val="729547"/>
+        <c:axId val="56648479"/>
+        <c:axId val="87619279"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50364798"/>
+        <c:axId val="56648479"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2611,12 +2677,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="729547"/>
+        <c:crossAx val="87619279"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="729547"/>
+        <c:axId val="87619279"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2675,7 +2741,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="50364798"/>
+        <c:crossAx val="56648479"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2702,7 +2768,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2943,11 +3009,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="75625677"/>
-        <c:axId val="38550363"/>
+        <c:axId val="4097130"/>
+        <c:axId val="7645868"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="75625677"/>
+        <c:axId val="4097130"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2975,12 +3041,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="38550363"/>
+        <c:crossAx val="7645868"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="38550363"/>
+        <c:axId val="7645868"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3017,7 +3083,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75625677"/>
+        <c:crossAx val="4097130"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3044,7 +3110,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3285,11 +3351,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="77682646"/>
-        <c:axId val="61269987"/>
+        <c:axId val="85998983"/>
+        <c:axId val="97661782"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="77682646"/>
+        <c:axId val="85998983"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3317,12 +3383,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61269987"/>
+        <c:crossAx val="97661782"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="61269987"/>
+        <c:axId val="97661782"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3359,7 +3425,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77682646"/>
+        <c:crossAx val="85998983"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3386,7 +3452,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -4428,11 +4494,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="91897255"/>
-        <c:axId val="66006209"/>
+        <c:axId val="70163219"/>
+        <c:axId val="91392776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="91897255"/>
+        <c:axId val="70163219"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4482,12 +4548,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="66006209"/>
+        <c:crossAx val="91392776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="66006209"/>
+        <c:axId val="91392776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4546,7 +4612,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="91897255"/>
+        <c:crossAx val="70163219"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4577,13 +4643,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
+      <xdr:col>19</xdr:col>
       <xdr:colOff>20160</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>86760</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
+      <xdr:col>37</xdr:col>
       <xdr:colOff>930240</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>75960</xdr:rowOff>
@@ -4594,8 +4660,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15113160" y="1544040"/>
-        <a:ext cx="15604200" cy="3227400"/>
+        <a:off x="15553440" y="1544040"/>
+        <a:ext cx="15603840" cy="3227400"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4607,13 +4673,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>808920</xdr:colOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>809280</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>64800</xdr:rowOff>
+      <xdr:rowOff>65160</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
+      <xdr:col>37</xdr:col>
       <xdr:colOff>907200</xdr:colOff>
       <xdr:row>50</xdr:row>
       <xdr:rowOff>64800</xdr:rowOff>
@@ -4624,8 +4690,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="15085440" y="4922280"/>
-        <a:ext cx="15608880" cy="3238560"/>
+        <a:off x="15525720" y="4922640"/>
+        <a:ext cx="15608520" cy="3238200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4637,13 +4703,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>24120</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>24480</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>74520</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>448200</xdr:colOff>
       <xdr:row>29</xdr:row>
       <xdr:rowOff>74880</xdr:rowOff>
@@ -4654,8 +4720,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8588160" y="1531800"/>
-        <a:ext cx="6136560" cy="3238560"/>
+        <a:off x="9028440" y="1531800"/>
+        <a:ext cx="6136200" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4667,13 +4733,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>14040</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>14400</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>159480</xdr:rowOff>
+      <xdr:rowOff>159840</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
+      <xdr:col>18</xdr:col>
       <xdr:colOff>566280</xdr:colOff>
       <xdr:row>49</xdr:row>
       <xdr:rowOff>159480</xdr:rowOff>
@@ -4684,8 +4750,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8578080" y="4854960"/>
-        <a:ext cx="6264720" cy="3238560"/>
+        <a:off x="9018360" y="4855320"/>
+        <a:ext cx="6264360" cy="3238200"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4697,13 +4763,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>360</xdr:colOff>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>720</xdr:colOff>
       <xdr:row>58</xdr:row>
-      <xdr:rowOff>45360</xdr:rowOff>
+      <xdr:rowOff>45720</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>30</xdr:col>
+      <xdr:col>31</xdr:col>
       <xdr:colOff>473040</xdr:colOff>
       <xdr:row>78</xdr:row>
       <xdr:rowOff>45720</xdr:rowOff>
@@ -4714,8 +4780,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="8564400" y="9436680"/>
-        <a:ext cx="15588360" cy="3238920"/>
+        <a:off x="9004680" y="9437040"/>
+        <a:ext cx="15588000" cy="3238560"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4733,13 +4799,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z166"/>
+  <dimension ref="A1:AA166"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I4" activeCellId="0" sqref="I4"/>
+      <selection pane="topLeft" activeCell="K11" activeCellId="0" sqref="K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="11.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.92"/>
@@ -4748,13 +4814,14 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="7.49"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="8" min="7" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="16.53"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.57"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="1" width="11.52"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="20" min="13" style="1" width="11.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="21" style="1" width="8.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="29" style="1" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.25"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="11.57"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="13" min="13" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="21" min="14" style="1" width="11.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="22" style="1" width="8.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="30" style="1" width="14.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -4769,16 +4836,17 @@
       <c r="G1" s="2"/>
       <c r="H1" s="2"/>
       <c r="I1" s="3"/>
-      <c r="J1" s="4" t="s">
+      <c r="J1" s="3"/>
+      <c r="K1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="4"/>
       <c r="L1" s="4"/>
       <c r="M1" s="4"/>
       <c r="N1" s="4"/>
       <c r="O1" s="4"/>
       <c r="P1" s="4"/>
       <c r="Q1" s="4"/>
+      <c r="R1" s="4"/>
     </row>
     <row r="2" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0"/>
@@ -4790,17 +4858,17 @@
       <c r="G2" s="0"/>
       <c r="H2" s="0"/>
       <c r="I2" s="3"/>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="3"/>
+      <c r="K2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="K2" s="4"/>
       <c r="L2" s="4"/>
       <c r="M2" s="4"/>
       <c r="N2" s="4"/>
       <c r="O2" s="4"/>
       <c r="P2" s="4"/>
       <c r="Q2" s="4"/>
-      <c r="R2" s="0"/>
+      <c r="R2" s="4"/>
       <c r="S2" s="0"/>
       <c r="T2" s="0"/>
       <c r="U2" s="0"/>
@@ -4809,6 +4877,7 @@
       <c r="X2" s="0"/>
       <c r="Y2" s="0"/>
       <c r="Z2" s="0"/>
+      <c r="AA2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0"/>
@@ -4819,17 +4888,16 @@
       <c r="F3" s="0"/>
       <c r="G3" s="0"/>
       <c r="H3" s="0"/>
-      <c r="J3" s="4" t="s">
+      <c r="K3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="K3" s="4"/>
       <c r="L3" s="4"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
       <c r="P3" s="4"/>
       <c r="Q3" s="4"/>
-      <c r="R3" s="0"/>
+      <c r="R3" s="4"/>
       <c r="S3" s="0"/>
       <c r="T3" s="0"/>
       <c r="U3" s="0"/>
@@ -4838,6 +4906,7 @@
       <c r="X3" s="0"/>
       <c r="Y3" s="0"/>
       <c r="Z3" s="0"/>
+      <c r="AA3" s="0"/>
     </row>
     <row r="4" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="5" t="s">
@@ -4854,17 +4923,16 @@
         <v>6</v>
       </c>
       <c r="H4" s="6"/>
-      <c r="J4" s="4" t="s">
+      <c r="K4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="4"/>
       <c r="L4" s="4"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
       <c r="P4" s="4"/>
       <c r="Q4" s="4"/>
-      <c r="R4" s="0"/>
+      <c r="R4" s="4"/>
       <c r="S4" s="0"/>
       <c r="T4" s="0"/>
       <c r="U4" s="0"/>
@@ -4873,6 +4941,7 @@
       <c r="X4" s="0"/>
       <c r="Y4" s="0"/>
       <c r="Z4" s="0"/>
+      <c r="AA4" s="0"/>
     </row>
     <row r="5" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="5" t="s">
@@ -4896,17 +4965,17 @@
         <v>9</v>
       </c>
       <c r="I5" s="0"/>
-      <c r="J5" s="4" t="s">
+      <c r="J5" s="0"/>
+      <c r="K5" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="K5" s="4"/>
       <c r="L5" s="4"/>
       <c r="M5" s="4"/>
       <c r="N5" s="4"/>
       <c r="O5" s="4"/>
       <c r="P5" s="4"/>
       <c r="Q5" s="4"/>
-      <c r="R5" s="0"/>
+      <c r="R5" s="4"/>
       <c r="S5" s="0"/>
       <c r="T5" s="0"/>
       <c r="U5" s="0"/>
@@ -4915,6 +4984,7 @@
       <c r="X5" s="0"/>
       <c r="Y5" s="0"/>
       <c r="Z5" s="0"/>
+      <c r="AA5" s="0"/>
     </row>
     <row r="6" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="7" t="n">
@@ -4923,19 +4993,20 @@
       <c r="B6" s="7" t="n">
         <v>18</v>
       </c>
-      <c r="D6" s="1" t="n">
+      <c r="C6" s="8"/>
+      <c r="D6" s="8" t="n">
         <v>0</v>
       </c>
-      <c r="E6" s="1" t="n">
+      <c r="E6" s="8" t="n">
         <v>18</v>
       </c>
+      <c r="F6" s="8"/>
       <c r="G6" s="7" t="n">
         <v>0</v>
       </c>
       <c r="H6" s="7" t="n">
         <v>705</v>
       </c>
-      <c r="M6" s="0"/>
       <c r="N6" s="0"/>
       <c r="O6" s="0"/>
       <c r="P6" s="0"/>
@@ -4949,6 +5020,7 @@
       <c r="X6" s="0"/>
       <c r="Y6" s="0"/>
       <c r="Z6" s="0"/>
+      <c r="AA6" s="0"/>
     </row>
     <row r="7" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="7" t="n">
@@ -4957,12 +5029,14 @@
       <c r="B7" s="7" t="n">
         <v>70</v>
       </c>
-      <c r="D7" s="1" t="n">
+      <c r="C7" s="8"/>
+      <c r="D7" s="8" t="n">
         <v>12</v>
       </c>
-      <c r="E7" s="1" t="n">
+      <c r="E7" s="8" t="n">
         <v>72</v>
       </c>
+      <c r="F7" s="8"/>
       <c r="G7" s="7" t="n">
         <v>12</v>
       </c>
@@ -4977,13 +5051,15 @@
       <c r="B8" s="7" t="n">
         <v>101</v>
       </c>
-      <c r="D8" s="1" t="n">
+      <c r="C8" s="8"/>
+      <c r="D8" s="8" t="n">
         <v>24</v>
       </c>
-      <c r="E8" s="1" t="n">
+      <c r="E8" s="8" t="n">
         <v>110</v>
       </c>
-      <c r="G8" s="0" t="n">
+      <c r="F8" s="8"/>
+      <c r="G8" s="8" t="n">
         <v>24</v>
       </c>
       <c r="H8" s="7" t="n">
@@ -4997,19 +5073,21 @@
       <c r="B9" s="7" t="n">
         <v>122</v>
       </c>
-      <c r="D9" s="1" t="n">
+      <c r="C9" s="8"/>
+      <c r="D9" s="8" t="n">
         <v>36</v>
       </c>
-      <c r="E9" s="1" t="n">
+      <c r="E9" s="8" t="n">
         <v>139</v>
       </c>
+      <c r="F9" s="8"/>
       <c r="G9" s="7" t="n">
         <v>36</v>
       </c>
       <c r="H9" s="7" t="n">
         <v>705</v>
       </c>
-      <c r="K9" s="7" t="s">
+      <c r="L9" s="9" t="s">
         <v>11</v>
       </c>
     </row>
@@ -5020,12 +5098,14 @@
       <c r="B10" s="7" t="n">
         <v>176</v>
       </c>
-      <c r="D10" s="1" t="n">
+      <c r="C10" s="8"/>
+      <c r="D10" s="8" t="n">
         <v>48</v>
       </c>
-      <c r="E10" s="1" t="n">
+      <c r="E10" s="8" t="n">
         <v>162</v>
       </c>
+      <c r="F10" s="8"/>
       <c r="G10" s="7" t="n">
         <v>48</v>
       </c>
@@ -5040,12 +5120,14 @@
       <c r="B11" s="7" t="n">
         <v>199</v>
       </c>
-      <c r="D11" s="1" t="n">
+      <c r="C11" s="8"/>
+      <c r="D11" s="8" t="n">
         <v>60</v>
       </c>
-      <c r="E11" s="1" t="n">
+      <c r="E11" s="8" t="n">
         <v>182</v>
       </c>
+      <c r="F11" s="8"/>
       <c r="G11" s="7" t="n">
         <v>60</v>
       </c>
@@ -5060,12 +5142,14 @@
       <c r="B12" s="7" t="n">
         <v>218</v>
       </c>
-      <c r="D12" s="1" t="n">
+      <c r="C12" s="8"/>
+      <c r="D12" s="8" t="n">
         <v>72</v>
       </c>
-      <c r="E12" s="1" t="n">
+      <c r="E12" s="8" t="n">
         <v>200</v>
       </c>
+      <c r="F12" s="8"/>
       <c r="G12" s="7" t="n">
         <v>72</v>
       </c>
@@ -5080,12 +5164,14 @@
       <c r="B13" s="7" t="n">
         <v>233</v>
       </c>
-      <c r="D13" s="1" t="n">
+      <c r="C13" s="8"/>
+      <c r="D13" s="8" t="n">
         <v>84</v>
       </c>
-      <c r="E13" s="1" t="n">
+      <c r="E13" s="8" t="n">
         <v>215</v>
       </c>
+      <c r="F13" s="8"/>
       <c r="G13" s="7" t="n">
         <v>84</v>
       </c>
@@ -5100,12 +5186,14 @@
       <c r="B14" s="7" t="n">
         <v>245</v>
       </c>
-      <c r="D14" s="1" t="n">
+      <c r="C14" s="8"/>
+      <c r="D14" s="8" t="n">
         <v>96</v>
       </c>
-      <c r="E14" s="1" t="n">
+      <c r="E14" s="8" t="n">
         <v>230</v>
       </c>
+      <c r="F14" s="8"/>
       <c r="G14" s="7" t="n">
         <v>96</v>
       </c>
@@ -5120,12 +5208,14 @@
       <c r="B15" s="7" t="n">
         <v>255</v>
       </c>
-      <c r="D15" s="1" t="n">
+      <c r="C15" s="8"/>
+      <c r="D15" s="8" t="n">
         <v>108</v>
       </c>
-      <c r="E15" s="1" t="n">
+      <c r="E15" s="8" t="n">
         <v>243</v>
       </c>
+      <c r="F15" s="8"/>
       <c r="G15" s="7" t="n">
         <v>108</v>
       </c>
@@ -5140,12 +5230,14 @@
       <c r="B16" s="7" t="n">
         <v>263</v>
       </c>
-      <c r="D16" s="1" t="n">
+      <c r="C16" s="8"/>
+      <c r="D16" s="8" t="n">
         <v>120</v>
       </c>
-      <c r="E16" s="1" t="n">
+      <c r="E16" s="8" t="n">
         <v>256</v>
       </c>
+      <c r="F16" s="8"/>
       <c r="G16" s="7" t="n">
         <v>120</v>
       </c>
@@ -5160,12 +5252,14 @@
       <c r="B17" s="7" t="n">
         <v>269</v>
       </c>
-      <c r="D17" s="1" t="n">
+      <c r="C17" s="8"/>
+      <c r="D17" s="8" t="n">
         <v>132</v>
       </c>
-      <c r="E17" s="1" t="n">
+      <c r="E17" s="8" t="n">
         <v>267</v>
       </c>
+      <c r="F17" s="8"/>
       <c r="G17" s="7" t="n">
         <v>132</v>
       </c>
@@ -5180,12 +5274,14 @@
       <c r="B18" s="7" t="n">
         <v>274</v>
       </c>
-      <c r="D18" s="1" t="n">
+      <c r="C18" s="8"/>
+      <c r="D18" s="8" t="n">
         <v>144</v>
       </c>
-      <c r="E18" s="1" t="n">
+      <c r="E18" s="8" t="n">
         <v>279</v>
       </c>
+      <c r="F18" s="8"/>
       <c r="G18" s="7" t="n">
         <v>144</v>
       </c>
@@ -5200,12 +5296,14 @@
       <c r="B19" s="7" t="n">
         <v>277</v>
       </c>
-      <c r="D19" s="1" t="n">
+      <c r="C19" s="8"/>
+      <c r="D19" s="8" t="n">
         <v>156</v>
       </c>
-      <c r="E19" s="1" t="n">
+      <c r="E19" s="8" t="n">
         <v>289</v>
       </c>
+      <c r="F19" s="8"/>
       <c r="G19" s="7" t="n">
         <v>156</v>
       </c>
@@ -5220,12 +5318,14 @@
       <c r="B20" s="7" t="n">
         <v>280</v>
       </c>
-      <c r="D20" s="1" t="n">
+      <c r="C20" s="8"/>
+      <c r="D20" s="8" t="n">
         <v>168</v>
       </c>
-      <c r="E20" s="1" t="n">
+      <c r="E20" s="8" t="n">
         <v>299</v>
       </c>
+      <c r="F20" s="8"/>
       <c r="G20" s="7" t="n">
         <v>168</v>
       </c>
@@ -5240,12 +5340,14 @@
       <c r="B21" s="7" t="n">
         <v>282</v>
       </c>
-      <c r="D21" s="1" t="n">
+      <c r="C21" s="8"/>
+      <c r="D21" s="8" t="n">
         <v>180</v>
       </c>
-      <c r="E21" s="1" t="n">
+      <c r="E21" s="8" t="n">
         <v>309</v>
       </c>
+      <c r="F21" s="8"/>
       <c r="G21" s="7" t="n">
         <v>180</v>
       </c>
@@ -5260,12 +5362,14 @@
       <c r="B22" s="7" t="n">
         <v>283</v>
       </c>
-      <c r="D22" s="1" t="n">
+      <c r="C22" s="8"/>
+      <c r="D22" s="8" t="n">
         <v>192</v>
       </c>
-      <c r="E22" s="1" t="n">
+      <c r="E22" s="8" t="n">
         <v>319</v>
       </c>
+      <c r="F22" s="8"/>
       <c r="G22" s="7" t="n">
         <v>192</v>
       </c>
@@ -5280,12 +5384,14 @@
       <c r="B23" s="7" t="n">
         <v>284</v>
       </c>
-      <c r="D23" s="1" t="n">
+      <c r="C23" s="8"/>
+      <c r="D23" s="8" t="n">
         <v>204</v>
       </c>
-      <c r="E23" s="1" t="n">
+      <c r="E23" s="8" t="n">
         <v>328</v>
       </c>
+      <c r="F23" s="8"/>
       <c r="G23" s="7" t="n">
         <v>204</v>
       </c>
@@ -5300,12 +5406,14 @@
       <c r="B24" s="7" t="n">
         <v>284</v>
       </c>
-      <c r="D24" s="1" t="n">
+      <c r="C24" s="8"/>
+      <c r="D24" s="8" t="n">
         <v>216</v>
       </c>
-      <c r="E24" s="1" t="n">
+      <c r="E24" s="8" t="n">
         <v>337</v>
       </c>
+      <c r="F24" s="8"/>
       <c r="G24" s="7" t="n">
         <v>216</v>
       </c>
@@ -5320,12 +5428,14 @@
       <c r="B25" s="7" t="n">
         <v>283</v>
       </c>
-      <c r="D25" s="1" t="n">
+      <c r="C25" s="8"/>
+      <c r="D25" s="8" t="n">
         <v>228</v>
       </c>
-      <c r="E25" s="1" t="n">
+      <c r="E25" s="8" t="n">
         <v>345</v>
       </c>
+      <c r="F25" s="8"/>
       <c r="G25" s="7" t="n">
         <v>228</v>
       </c>
@@ -5340,12 +5450,14 @@
       <c r="B26" s="7" t="n">
         <v>283</v>
       </c>
-      <c r="D26" s="1" t="n">
+      <c r="C26" s="8"/>
+      <c r="D26" s="8" t="n">
         <v>240</v>
       </c>
-      <c r="E26" s="1" t="n">
+      <c r="E26" s="8" t="n">
         <v>354</v>
       </c>
+      <c r="F26" s="8"/>
       <c r="G26" s="7" t="n">
         <v>240</v>
       </c>
@@ -5360,12 +5472,14 @@
       <c r="B27" s="7" t="n">
         <v>282</v>
       </c>
-      <c r="D27" s="1" t="n">
+      <c r="C27" s="8"/>
+      <c r="D27" s="8" t="n">
         <v>252</v>
       </c>
-      <c r="E27" s="1" t="n">
+      <c r="E27" s="8" t="n">
         <v>362</v>
       </c>
+      <c r="F27" s="8"/>
       <c r="G27" s="7" t="n">
         <v>252</v>
       </c>
@@ -5380,12 +5494,14 @@
       <c r="B28" s="7" t="n">
         <v>280</v>
       </c>
-      <c r="D28" s="1" t="n">
+      <c r="C28" s="8"/>
+      <c r="D28" s="8" t="n">
         <v>264</v>
       </c>
-      <c r="E28" s="1" t="n">
+      <c r="E28" s="8" t="n">
         <v>370</v>
       </c>
+      <c r="F28" s="8"/>
       <c r="G28" s="7" t="n">
         <v>264</v>
       </c>
@@ -5400,12 +5516,14 @@
       <c r="B29" s="7" t="n">
         <v>279</v>
       </c>
-      <c r="D29" s="1" t="n">
+      <c r="C29" s="8"/>
+      <c r="D29" s="8" t="n">
         <v>276</v>
       </c>
-      <c r="E29" s="1" t="n">
+      <c r="E29" s="8" t="n">
         <v>377</v>
       </c>
+      <c r="F29" s="8"/>
       <c r="G29" s="7" t="n">
         <v>276</v>
       </c>
@@ -5420,12 +5538,14 @@
       <c r="B30" s="7" t="n">
         <v>277</v>
       </c>
-      <c r="D30" s="1" t="n">
+      <c r="C30" s="8"/>
+      <c r="D30" s="8" t="n">
         <v>288</v>
       </c>
-      <c r="E30" s="1" t="n">
+      <c r="E30" s="8" t="n">
         <v>385</v>
       </c>
+      <c r="F30" s="8"/>
       <c r="G30" s="7" t="n">
         <v>288</v>
       </c>
@@ -5434,826 +5554,904 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="7" t="n">
+      <c r="A31" s="10" t="n">
         <v>300</v>
       </c>
-      <c r="B31" s="7" t="n">
+      <c r="B31" s="10" t="n">
         <v>376</v>
       </c>
-      <c r="D31" s="1" t="n">
+      <c r="C31" s="11"/>
+      <c r="D31" s="11" t="n">
         <v>300</v>
       </c>
-      <c r="E31" s="1" t="n">
+      <c r="E31" s="11" t="n">
         <v>388</v>
       </c>
-      <c r="G31" s="7" t="n">
+      <c r="F31" s="11"/>
+      <c r="G31" s="10" t="n">
         <v>300</v>
       </c>
-      <c r="H31" s="7" t="n">
+      <c r="H31" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="7" t="n">
+      <c r="A32" s="10" t="n">
         <v>4779</v>
       </c>
-      <c r="B32" s="7" t="n">
+      <c r="B32" s="10" t="n">
         <v>460</v>
       </c>
-      <c r="D32" s="1" t="n">
+      <c r="C32" s="11"/>
+      <c r="D32" s="11" t="n">
         <v>4779</v>
       </c>
-      <c r="E32" s="1" t="n">
+      <c r="E32" s="11" t="n">
         <v>381</v>
       </c>
-      <c r="G32" s="7" t="n">
+      <c r="F32" s="11"/>
+      <c r="G32" s="10" t="n">
         <v>4779</v>
       </c>
-      <c r="H32" s="7" t="n">
+      <c r="H32" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="7" t="n">
+      <c r="A33" s="10" t="n">
         <v>9258</v>
       </c>
-      <c r="B33" s="7" t="n">
+      <c r="B33" s="10" t="n">
         <v>449</v>
       </c>
-      <c r="D33" s="1" t="n">
+      <c r="C33" s="11"/>
+      <c r="D33" s="11" t="n">
         <v>9258</v>
       </c>
-      <c r="E33" s="1" t="n">
+      <c r="E33" s="11" t="n">
         <v>373</v>
       </c>
-      <c r="G33" s="7" t="n">
+      <c r="F33" s="11"/>
+      <c r="G33" s="10" t="n">
         <v>9258</v>
       </c>
-      <c r="H33" s="7" t="n">
+      <c r="H33" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="7" t="n">
+      <c r="A34" s="10" t="n">
         <v>13737</v>
       </c>
-      <c r="B34" s="7" t="n">
+      <c r="B34" s="10" t="n">
         <v>439</v>
       </c>
-      <c r="D34" s="1" t="n">
+      <c r="C34" s="11"/>
+      <c r="D34" s="11" t="n">
         <v>13737</v>
       </c>
-      <c r="E34" s="1" t="n">
+      <c r="E34" s="11" t="n">
         <v>366</v>
       </c>
-      <c r="G34" s="7" t="n">
+      <c r="F34" s="11"/>
+      <c r="G34" s="10" t="n">
         <v>13737</v>
       </c>
-      <c r="H34" s="7" t="n">
+      <c r="H34" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="7" t="n">
+      <c r="A35" s="10" t="n">
         <v>18216</v>
       </c>
-      <c r="B35" s="7" t="n">
+      <c r="B35" s="10" t="n">
         <v>429</v>
       </c>
-      <c r="D35" s="1" t="n">
+      <c r="C35" s="11"/>
+      <c r="D35" s="11" t="n">
         <v>18216</v>
       </c>
-      <c r="E35" s="1" t="n">
+      <c r="E35" s="11" t="n">
         <v>359</v>
       </c>
-      <c r="G35" s="7" t="n">
+      <c r="F35" s="11"/>
+      <c r="G35" s="10" t="n">
         <v>18216</v>
       </c>
-      <c r="H35" s="7" t="n">
+      <c r="H35" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="7" t="n">
+      <c r="A36" s="10" t="n">
         <v>22695</v>
       </c>
-      <c r="B36" s="7" t="n">
+      <c r="B36" s="10" t="n">
         <v>420</v>
       </c>
-      <c r="D36" s="1" t="n">
+      <c r="C36" s="11"/>
+      <c r="D36" s="11" t="n">
         <v>22695</v>
       </c>
-      <c r="E36" s="1" t="n">
+      <c r="E36" s="11" t="n">
         <v>353</v>
       </c>
-      <c r="G36" s="7" t="n">
+      <c r="F36" s="11"/>
+      <c r="G36" s="10" t="n">
         <v>22695</v>
       </c>
-      <c r="H36" s="7" t="n">
+      <c r="H36" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="7" t="n">
+      <c r="A37" s="10" t="n">
         <v>27174</v>
       </c>
-      <c r="B37" s="7" t="n">
+      <c r="B37" s="10" t="n">
         <v>411</v>
       </c>
-      <c r="D37" s="1" t="n">
+      <c r="C37" s="11"/>
+      <c r="D37" s="11" t="n">
         <v>27174</v>
       </c>
-      <c r="E37" s="1" t="n">
+      <c r="E37" s="11" t="n">
         <v>347</v>
       </c>
-      <c r="G37" s="7" t="n">
+      <c r="F37" s="11"/>
+      <c r="G37" s="10" t="n">
         <v>27174</v>
       </c>
-      <c r="H37" s="7" t="n">
+      <c r="H37" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="7" t="n">
+      <c r="A38" s="10" t="n">
         <v>31653</v>
       </c>
-      <c r="B38" s="7" t="n">
+      <c r="B38" s="10" t="n">
         <v>402</v>
       </c>
-      <c r="D38" s="1" t="n">
+      <c r="C38" s="11"/>
+      <c r="D38" s="11" t="n">
         <v>31653</v>
       </c>
-      <c r="E38" s="1" t="n">
+      <c r="E38" s="11" t="n">
         <v>341</v>
       </c>
-      <c r="G38" s="7" t="n">
+      <c r="F38" s="11"/>
+      <c r="G38" s="10" t="n">
         <v>31653</v>
       </c>
-      <c r="H38" s="7" t="n">
+      <c r="H38" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="7" t="n">
+      <c r="A39" s="10" t="n">
         <v>36132</v>
       </c>
-      <c r="B39" s="7" t="n">
+      <c r="B39" s="10" t="n">
         <v>394</v>
       </c>
-      <c r="D39" s="1" t="n">
+      <c r="C39" s="11"/>
+      <c r="D39" s="11" t="n">
         <v>36132</v>
       </c>
-      <c r="E39" s="1" t="n">
+      <c r="E39" s="11" t="n">
         <v>336</v>
       </c>
-      <c r="G39" s="7" t="n">
+      <c r="F39" s="11"/>
+      <c r="G39" s="10" t="n">
         <v>36132</v>
       </c>
-      <c r="H39" s="7" t="n">
+      <c r="H39" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="7" t="n">
+      <c r="A40" s="10" t="n">
         <v>40611</v>
       </c>
-      <c r="B40" s="7" t="n">
+      <c r="B40" s="10" t="n">
         <v>386</v>
       </c>
-      <c r="D40" s="1" t="n">
+      <c r="C40" s="11"/>
+      <c r="D40" s="11" t="n">
         <v>40611</v>
       </c>
-      <c r="E40" s="1" t="n">
+      <c r="E40" s="11" t="n">
         <v>331</v>
       </c>
-      <c r="G40" s="7" t="n">
+      <c r="F40" s="11"/>
+      <c r="G40" s="10" t="n">
         <v>40611</v>
       </c>
-      <c r="H40" s="7" t="n">
+      <c r="H40" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="7" t="n">
+      <c r="A41" s="10" t="n">
         <v>45090</v>
       </c>
-      <c r="B41" s="7" t="n">
+      <c r="B41" s="10" t="n">
         <v>378</v>
       </c>
-      <c r="D41" s="1" t="n">
+      <c r="C41" s="11"/>
+      <c r="D41" s="11" t="n">
         <v>45090</v>
       </c>
-      <c r="E41" s="1" t="n">
+      <c r="E41" s="11" t="n">
         <v>326</v>
       </c>
-      <c r="G41" s="7" t="n">
+      <c r="F41" s="11"/>
+      <c r="G41" s="10" t="n">
         <v>45090</v>
       </c>
-      <c r="H41" s="7" t="n">
+      <c r="H41" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="7" t="n">
+      <c r="A42" s="10" t="n">
         <v>49569</v>
       </c>
-      <c r="B42" s="7" t="n">
+      <c r="B42" s="10" t="n">
         <v>370</v>
       </c>
-      <c r="D42" s="1" t="n">
+      <c r="C42" s="11"/>
+      <c r="D42" s="11" t="n">
         <v>49569</v>
       </c>
-      <c r="E42" s="1" t="n">
+      <c r="E42" s="11" t="n">
         <v>321</v>
       </c>
-      <c r="G42" s="7" t="n">
+      <c r="F42" s="11"/>
+      <c r="G42" s="10" t="n">
         <v>49569</v>
       </c>
-      <c r="H42" s="7" t="n">
+      <c r="H42" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="7" t="n">
+      <c r="A43" s="10" t="n">
         <v>54048</v>
       </c>
-      <c r="B43" s="7" t="n">
+      <c r="B43" s="10" t="n">
         <v>362</v>
       </c>
-      <c r="D43" s="1" t="n">
+      <c r="C43" s="11"/>
+      <c r="D43" s="11" t="n">
         <v>54048</v>
       </c>
-      <c r="E43" s="1" t="n">
+      <c r="E43" s="11" t="n">
         <v>316</v>
       </c>
-      <c r="G43" s="7" t="n">
+      <c r="F43" s="11"/>
+      <c r="G43" s="10" t="n">
         <v>54048</v>
       </c>
-      <c r="H43" s="7" t="n">
+      <c r="H43" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="7" t="n">
+      <c r="A44" s="10" t="n">
         <v>58527</v>
       </c>
-      <c r="B44" s="7" t="n">
+      <c r="B44" s="10" t="n">
         <v>355</v>
       </c>
-      <c r="D44" s="1" t="n">
+      <c r="C44" s="11"/>
+      <c r="D44" s="11" t="n">
         <v>58527</v>
       </c>
-      <c r="E44" s="1" t="n">
+      <c r="E44" s="11" t="n">
         <v>312</v>
       </c>
-      <c r="G44" s="7" t="n">
+      <c r="F44" s="11"/>
+      <c r="G44" s="10" t="n">
         <v>58527</v>
       </c>
-      <c r="H44" s="7" t="n">
+      <c r="H44" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="7" t="n">
+      <c r="A45" s="10" t="n">
         <v>63006</v>
       </c>
-      <c r="B45" s="7" t="n">
+      <c r="B45" s="10" t="n">
         <v>348</v>
       </c>
-      <c r="D45" s="1" t="n">
+      <c r="C45" s="11"/>
+      <c r="D45" s="11" t="n">
         <v>63006</v>
       </c>
-      <c r="E45" s="1" t="n">
+      <c r="E45" s="11" t="n">
         <v>308</v>
       </c>
-      <c r="G45" s="7" t="n">
+      <c r="F45" s="11"/>
+      <c r="G45" s="10" t="n">
         <v>63006</v>
       </c>
-      <c r="H45" s="7" t="n">
+      <c r="H45" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="7" t="n">
+      <c r="A46" s="10" t="n">
         <v>67485</v>
       </c>
-      <c r="B46" s="7" t="n">
+      <c r="B46" s="10" t="n">
         <v>341</v>
       </c>
-      <c r="D46" s="1" t="n">
+      <c r="C46" s="11"/>
+      <c r="D46" s="11" t="n">
         <v>67485</v>
       </c>
-      <c r="E46" s="1" t="n">
+      <c r="E46" s="11" t="n">
         <v>304</v>
       </c>
-      <c r="G46" s="7" t="n">
+      <c r="F46" s="11"/>
+      <c r="G46" s="10" t="n">
         <v>67485</v>
       </c>
-      <c r="H46" s="7" t="n">
+      <c r="H46" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="7" t="n">
+      <c r="A47" s="10" t="n">
         <v>71964</v>
       </c>
-      <c r="B47" s="7" t="n">
+      <c r="B47" s="10" t="n">
         <v>334</v>
       </c>
-      <c r="D47" s="1" t="n">
+      <c r="C47" s="11"/>
+      <c r="D47" s="11" t="n">
         <v>71964</v>
       </c>
-      <c r="E47" s="1" t="n">
+      <c r="E47" s="11" t="n">
         <v>300</v>
       </c>
-      <c r="G47" s="7" t="n">
+      <c r="F47" s="11"/>
+      <c r="G47" s="10" t="n">
         <v>71964</v>
       </c>
-      <c r="H47" s="7" t="n">
+      <c r="H47" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="7" t="n">
+      <c r="A48" s="10" t="n">
         <v>76443</v>
       </c>
-      <c r="B48" s="7" t="n">
+      <c r="B48" s="10" t="n">
         <v>328</v>
       </c>
-      <c r="D48" s="1" t="n">
+      <c r="C48" s="11"/>
+      <c r="D48" s="11" t="n">
         <v>76443</v>
       </c>
-      <c r="E48" s="1" t="n">
+      <c r="E48" s="11" t="n">
         <v>296</v>
       </c>
-      <c r="G48" s="7" t="n">
+      <c r="F48" s="11"/>
+      <c r="G48" s="10" t="n">
         <v>76443</v>
       </c>
-      <c r="H48" s="7" t="n">
+      <c r="H48" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="7" t="n">
+      <c r="A49" s="10" t="n">
         <v>80922</v>
       </c>
-      <c r="B49" s="7" t="n">
+      <c r="B49" s="10" t="n">
         <v>322</v>
       </c>
-      <c r="D49" s="1" t="n">
+      <c r="C49" s="11"/>
+      <c r="D49" s="11" t="n">
         <v>80922</v>
       </c>
-      <c r="E49" s="1" t="n">
+      <c r="E49" s="11" t="n">
         <v>293</v>
       </c>
-      <c r="G49" s="7" t="n">
+      <c r="F49" s="11"/>
+      <c r="G49" s="10" t="n">
         <v>80922</v>
       </c>
-      <c r="H49" s="7" t="n">
+      <c r="H49" s="10" t="n">
         <v>705</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="7" t="n">
+      <c r="A50" s="10" t="n">
         <v>85401</v>
       </c>
-      <c r="B50" s="7" t="n">
+      <c r="B50" s="10" t="n">
         <v>316</v>
       </c>
-      <c r="D50" s="1" t="n">
+      <c r="C50" s="11"/>
+      <c r="D50" s="11" t="n">
         <v>85401</v>
       </c>
-      <c r="E50" s="1" t="n">
+      <c r="E50" s="11" t="n">
         <v>289</v>
       </c>
-      <c r="G50" s="7" t="n">
+      <c r="F50" s="11"/>
+      <c r="G50" s="10" t="n">
         <v>85401</v>
       </c>
-      <c r="H50" s="7" t="n">
+      <c r="H50" s="10" t="n">
         <v>705</v>
       </c>
-      <c r="L50" s="0"/>
       <c r="M50" s="0"/>
       <c r="N50" s="0"/>
       <c r="O50" s="0"/>
+      <c r="P50" s="0"/>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="7" t="n">
+      <c r="A51" s="12" t="n">
         <v>89880</v>
       </c>
-      <c r="B51" s="7" t="n">
+      <c r="B51" s="12" t="n">
         <v>310</v>
       </c>
-      <c r="D51" s="1" t="n">
+      <c r="C51" s="13"/>
+      <c r="D51" s="13" t="n">
         <v>89880</v>
       </c>
-      <c r="E51" s="1" t="n">
+      <c r="E51" s="13" t="n">
         <v>286</v>
       </c>
-      <c r="G51" s="7" t="n">
+      <c r="F51" s="13"/>
+      <c r="G51" s="12" t="n">
         <v>89880</v>
       </c>
-      <c r="H51" s="7" t="n">
+      <c r="H51" s="12" t="n">
         <v>352</v>
       </c>
-      <c r="L51" s="0"/>
       <c r="M51" s="0"/>
       <c r="N51" s="0"/>
       <c r="O51" s="0"/>
+      <c r="P51" s="0"/>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="7" t="n">
+      <c r="A52" s="12" t="n">
         <v>94359</v>
       </c>
-      <c r="B52" s="7" t="n">
+      <c r="B52" s="12" t="n">
         <v>304</v>
       </c>
-      <c r="D52" s="1" t="n">
+      <c r="C52" s="13"/>
+      <c r="D52" s="13" t="n">
         <v>94359</v>
       </c>
-      <c r="E52" s="1" t="n">
+      <c r="E52" s="13" t="n">
         <v>282</v>
       </c>
-      <c r="G52" s="7" t="n">
+      <c r="F52" s="13"/>
+      <c r="G52" s="12" t="n">
         <v>94359</v>
       </c>
-      <c r="H52" s="7" t="n">
+      <c r="H52" s="12" t="n">
         <v>352</v>
       </c>
-      <c r="L52" s="0"/>
       <c r="M52" s="0"/>
       <c r="N52" s="0"/>
       <c r="O52" s="0"/>
+      <c r="P52" s="0"/>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="7" t="n">
+      <c r="A53" s="12" t="n">
         <v>98838</v>
       </c>
-      <c r="B53" s="7" t="n">
+      <c r="B53" s="12" t="n">
         <v>298</v>
       </c>
-      <c r="D53" s="1" t="n">
+      <c r="C53" s="13"/>
+      <c r="D53" s="13" t="n">
         <v>98838</v>
       </c>
-      <c r="E53" s="1" t="n">
+      <c r="E53" s="13" t="n">
         <v>279</v>
       </c>
-      <c r="G53" s="7" t="n">
+      <c r="F53" s="13"/>
+      <c r="G53" s="12" t="n">
         <v>98838</v>
       </c>
-      <c r="H53" s="7" t="n">
+      <c r="H53" s="12" t="n">
         <v>352</v>
       </c>
-      <c r="L53" s="0"/>
       <c r="M53" s="0"/>
       <c r="N53" s="0"/>
       <c r="O53" s="0"/>
+      <c r="P53" s="0"/>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="7" t="n">
+      <c r="A54" s="12" t="n">
         <v>103317</v>
       </c>
-      <c r="B54" s="7" t="n">
+      <c r="B54" s="12" t="n">
         <v>293</v>
       </c>
-      <c r="D54" s="1" t="n">
+      <c r="C54" s="13"/>
+      <c r="D54" s="13" t="n">
         <v>103317</v>
       </c>
-      <c r="E54" s="1" t="n">
+      <c r="E54" s="13" t="n">
         <v>276</v>
       </c>
-      <c r="G54" s="7" t="n">
+      <c r="F54" s="13"/>
+      <c r="G54" s="12" t="n">
         <v>103317</v>
       </c>
-      <c r="H54" s="7" t="n">
+      <c r="H54" s="12" t="n">
         <v>352</v>
       </c>
-      <c r="K54" s="1" t="s">
+      <c r="L54" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N54" s="0"/>
       <c r="O54" s="0"/>
+      <c r="P54" s="0"/>
     </row>
     <row r="55" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A55" s="7" t="n">
+      <c r="A55" s="12" t="n">
         <v>107796</v>
       </c>
-      <c r="B55" s="7" t="n">
+      <c r="B55" s="12" t="n">
         <v>288</v>
       </c>
-      <c r="D55" s="1" t="n">
+      <c r="C55" s="13"/>
+      <c r="D55" s="13" t="n">
         <v>107796</v>
       </c>
-      <c r="E55" s="1" t="n">
+      <c r="E55" s="13" t="n">
         <v>273</v>
       </c>
-      <c r="G55" s="7" t="n">
+      <c r="F55" s="13"/>
+      <c r="G55" s="12" t="n">
         <v>107796</v>
       </c>
-      <c r="H55" s="7" t="n">
+      <c r="H55" s="12" t="n">
         <v>352</v>
       </c>
-      <c r="L55" s="0"/>
       <c r="M55" s="0"/>
       <c r="N55" s="0"/>
       <c r="O55" s="0"/>
+      <c r="P55" s="0"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="7" t="n">
+      <c r="A56" s="12" t="n">
         <v>112275</v>
       </c>
-      <c r="B56" s="7" t="n">
+      <c r="B56" s="12" t="n">
         <v>282</v>
       </c>
-      <c r="D56" s="1" t="n">
+      <c r="C56" s="13"/>
+      <c r="D56" s="13" t="n">
         <v>112275</v>
       </c>
-      <c r="E56" s="1" t="n">
+      <c r="E56" s="13" t="n">
         <v>270</v>
       </c>
-      <c r="G56" s="7" t="n">
+      <c r="F56" s="13"/>
+      <c r="G56" s="12" t="n">
         <v>112275</v>
       </c>
-      <c r="H56" s="7" t="n">
+      <c r="H56" s="12" t="n">
         <v>352</v>
       </c>
-      <c r="K56" s="1" t="s">
+      <c r="L56" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N56" s="0"/>
       <c r="O56" s="0"/>
+      <c r="P56" s="0"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="7" t="n">
+      <c r="A57" s="12" t="n">
         <v>116754</v>
       </c>
-      <c r="B57" s="7" t="n">
+      <c r="B57" s="12" t="n">
         <v>277</v>
       </c>
-      <c r="D57" s="1" t="n">
+      <c r="C57" s="13"/>
+      <c r="D57" s="13" t="n">
         <v>116754</v>
       </c>
-      <c r="E57" s="1" t="n">
+      <c r="E57" s="13" t="n">
         <v>268</v>
       </c>
-      <c r="G57" s="7" t="n">
+      <c r="F57" s="13"/>
+      <c r="G57" s="12" t="n">
         <v>116754</v>
       </c>
-      <c r="H57" s="7" t="n">
+      <c r="H57" s="12" t="n">
         <v>352</v>
       </c>
-      <c r="K57" s="1" t="s">
+      <c r="L57" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="7" t="n">
+      <c r="A58" s="12" t="n">
         <v>121233</v>
       </c>
-      <c r="B58" s="7" t="n">
+      <c r="B58" s="12" t="n">
         <v>273</v>
       </c>
-      <c r="D58" s="1" t="n">
+      <c r="C58" s="13"/>
+      <c r="D58" s="13" t="n">
         <v>121233</v>
       </c>
-      <c r="E58" s="1" t="n">
+      <c r="E58" s="13" t="n">
         <v>265</v>
       </c>
-      <c r="G58" s="7" t="n">
+      <c r="F58" s="13"/>
+      <c r="G58" s="12" t="n">
         <v>121233</v>
       </c>
-      <c r="H58" s="7" t="n">
+      <c r="H58" s="12" t="n">
         <v>352</v>
       </c>
-      <c r="K58" s="1" t="s">
+      <c r="L58" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="7" t="n">
+      <c r="A59" s="12" t="n">
         <v>125712</v>
       </c>
-      <c r="B59" s="7" t="n">
+      <c r="B59" s="12" t="n">
         <v>268</v>
       </c>
-      <c r="D59" s="1" t="n">
+      <c r="C59" s="13"/>
+      <c r="D59" s="13" t="n">
         <v>125712</v>
       </c>
-      <c r="E59" s="1" t="n">
+      <c r="E59" s="13" t="n">
         <v>262</v>
       </c>
-      <c r="G59" s="7" t="n">
+      <c r="F59" s="13"/>
+      <c r="G59" s="12" t="n">
         <v>125712</v>
       </c>
-      <c r="H59" s="7" t="n">
+      <c r="H59" s="12" t="n">
         <v>352</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="7" t="n">
+      <c r="A60" s="12" t="n">
         <v>130191</v>
       </c>
-      <c r="B60" s="7" t="n">
+      <c r="B60" s="12" t="n">
         <v>263</v>
       </c>
-      <c r="D60" s="1" t="n">
+      <c r="C60" s="13"/>
+      <c r="D60" s="13" t="n">
         <v>130191</v>
       </c>
-      <c r="E60" s="1" t="n">
+      <c r="E60" s="13" t="n">
         <v>260</v>
       </c>
-      <c r="G60" s="7" t="n">
+      <c r="F60" s="13"/>
+      <c r="G60" s="12" t="n">
         <v>130191</v>
       </c>
-      <c r="H60" s="7" t="n">
+      <c r="H60" s="12" t="n">
         <v>352</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="7" t="n">
+      <c r="A61" s="12" t="n">
         <v>134670</v>
       </c>
-      <c r="B61" s="7" t="n">
+      <c r="B61" s="12" t="n">
         <v>259</v>
       </c>
-      <c r="D61" s="1" t="n">
+      <c r="C61" s="13"/>
+      <c r="D61" s="13" t="n">
         <v>134670</v>
       </c>
-      <c r="E61" s="1" t="n">
+      <c r="E61" s="13" t="n">
         <v>257</v>
       </c>
-      <c r="G61" s="7" t="n">
+      <c r="F61" s="13"/>
+      <c r="G61" s="12" t="n">
         <v>134670</v>
       </c>
-      <c r="H61" s="7" t="n">
+      <c r="H61" s="12" t="n">
         <v>352</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="7" t="n">
+      <c r="A62" s="12" t="n">
         <v>139149</v>
       </c>
-      <c r="B62" s="7" t="n">
+      <c r="B62" s="12" t="n">
         <v>254</v>
       </c>
-      <c r="D62" s="1" t="n">
+      <c r="C62" s="13"/>
+      <c r="D62" s="13" t="n">
         <v>139149</v>
       </c>
-      <c r="E62" s="1" t="n">
+      <c r="E62" s="13" t="n">
         <v>255</v>
       </c>
-      <c r="G62" s="7" t="n">
+      <c r="F62" s="13"/>
+      <c r="G62" s="12" t="n">
         <v>139149</v>
       </c>
-      <c r="H62" s="7" t="n">
+      <c r="H62" s="12" t="n">
         <v>352</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="7" t="n">
+      <c r="A63" s="12" t="n">
         <v>143628</v>
       </c>
-      <c r="B63" s="7" t="n">
+      <c r="B63" s="12" t="n">
         <v>250</v>
       </c>
-      <c r="D63" s="1" t="n">
+      <c r="C63" s="13"/>
+      <c r="D63" s="13" t="n">
         <v>143628</v>
       </c>
-      <c r="E63" s="1" t="n">
+      <c r="E63" s="13" t="n">
         <v>253</v>
       </c>
-      <c r="G63" s="7" t="n">
+      <c r="F63" s="13"/>
+      <c r="G63" s="12" t="n">
         <v>143628</v>
       </c>
-      <c r="H63" s="7" t="n">
+      <c r="H63" s="12" t="n">
         <v>352</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="7" t="n">
+      <c r="A64" s="12" t="n">
         <v>148107</v>
       </c>
-      <c r="B64" s="7" t="n">
+      <c r="B64" s="12" t="n">
         <v>246</v>
       </c>
-      <c r="D64" s="1" t="n">
+      <c r="C64" s="13"/>
+      <c r="D64" s="13" t="n">
         <v>148107</v>
       </c>
-      <c r="E64" s="1" t="n">
+      <c r="E64" s="13" t="n">
         <v>250</v>
       </c>
-      <c r="G64" s="7" t="n">
+      <c r="F64" s="13"/>
+      <c r="G64" s="12" t="n">
         <v>148107</v>
       </c>
-      <c r="H64" s="7" t="n">
+      <c r="H64" s="12" t="n">
         <v>352</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="7" t="n">
+      <c r="A65" s="12" t="n">
         <v>152586</v>
       </c>
-      <c r="B65" s="7" t="n">
+      <c r="B65" s="12" t="n">
         <v>242</v>
       </c>
-      <c r="D65" s="1" t="n">
+      <c r="C65" s="13"/>
+      <c r="D65" s="13" t="n">
         <v>152586</v>
       </c>
-      <c r="E65" s="1" t="n">
+      <c r="E65" s="13" t="n">
         <v>248</v>
       </c>
-      <c r="G65" s="7" t="n">
+      <c r="F65" s="13"/>
+      <c r="G65" s="12" t="n">
         <v>152586</v>
       </c>
-      <c r="H65" s="7" t="n">
+      <c r="H65" s="12" t="n">
         <v>352</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A66" s="7" t="n">
+      <c r="A66" s="12" t="n">
         <v>157065</v>
       </c>
-      <c r="B66" s="7" t="n">
+      <c r="B66" s="12" t="n">
         <v>238</v>
       </c>
-      <c r="D66" s="1" t="n">
+      <c r="C66" s="13"/>
+      <c r="D66" s="13" t="n">
         <v>157065</v>
       </c>
-      <c r="E66" s="1" t="n">
+      <c r="E66" s="13" t="n">
         <v>246</v>
       </c>
-      <c r="G66" s="7" t="n">
+      <c r="F66" s="13"/>
+      <c r="G66" s="12" t="n">
         <v>157065</v>
       </c>
-      <c r="H66" s="7" t="n">
+      <c r="H66" s="12" t="n">
         <v>352</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A67" s="7" t="n">
+      <c r="A67" s="12" t="n">
         <v>161544</v>
       </c>
-      <c r="B67" s="7" t="n">
+      <c r="B67" s="12" t="n">
         <v>234</v>
       </c>
-      <c r="D67" s="1" t="n">
+      <c r="C67" s="13"/>
+      <c r="D67" s="13" t="n">
         <v>161544</v>
       </c>
-      <c r="E67" s="1" t="n">
+      <c r="E67" s="13" t="n">
         <v>244</v>
       </c>
-      <c r="G67" s="7" t="n">
+      <c r="F67" s="13"/>
+      <c r="G67" s="12" t="n">
         <v>161544</v>
       </c>
-      <c r="H67" s="7" t="n">
+      <c r="H67" s="12" t="n">
         <v>352</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A68" s="7" t="n">
+      <c r="A68" s="12" t="n">
         <v>166023</v>
       </c>
-      <c r="B68" s="7" t="n">
+      <c r="B68" s="12" t="n">
         <v>230</v>
       </c>
-      <c r="D68" s="1" t="n">
+      <c r="C68" s="13"/>
+      <c r="D68" s="13" t="n">
         <v>166023</v>
       </c>
-      <c r="E68" s="1" t="n">
+      <c r="E68" s="13" t="n">
         <v>242</v>
       </c>
-      <c r="G68" s="7" t="n">
+      <c r="F68" s="13"/>
+      <c r="G68" s="12" t="n">
         <v>166023</v>
       </c>
-      <c r="H68" s="7" t="n">
+      <c r="H68" s="12" t="n">
         <v>352</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A69" s="7" t="n">
+      <c r="A69" s="12" t="n">
         <v>170502</v>
       </c>
-      <c r="B69" s="7" t="n">
+      <c r="B69" s="12" t="n">
         <v>226</v>
       </c>
-      <c r="D69" s="1" t="n">
+      <c r="C69" s="13"/>
+      <c r="D69" s="13" t="n">
         <v>170502</v>
       </c>
-      <c r="E69" s="1" t="n">
+      <c r="E69" s="13" t="n">
         <v>240</v>
       </c>
-      <c r="G69" s="7" t="n">
+      <c r="F69" s="13"/>
+      <c r="G69" s="12" t="n">
         <v>170502</v>
       </c>
-      <c r="H69" s="7" t="n">
+      <c r="H69" s="12" t="n">
         <v>352</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A70" s="7" t="n">
+      <c r="A70" s="9" t="n">
         <v>174981</v>
       </c>
-      <c r="B70" s="7" t="n">
+      <c r="B70" s="9" t="n">
         <v>223</v>
       </c>
       <c r="D70" s="1" t="n">
@@ -6262,18 +6460,18 @@
       <c r="E70" s="1" t="n">
         <v>238</v>
       </c>
-      <c r="G70" s="7" t="n">
+      <c r="G70" s="9" t="n">
         <v>174981</v>
       </c>
-      <c r="H70" s="7" t="n">
+      <c r="H70" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A71" s="7" t="n">
+      <c r="A71" s="9" t="n">
         <v>179460</v>
       </c>
-      <c r="B71" s="7" t="n">
+      <c r="B71" s="9" t="n">
         <v>219</v>
       </c>
       <c r="D71" s="1" t="n">
@@ -6282,18 +6480,18 @@
       <c r="E71" s="1" t="n">
         <v>236</v>
       </c>
-      <c r="G71" s="7" t="n">
+      <c r="G71" s="9" t="n">
         <v>179460</v>
       </c>
-      <c r="H71" s="7" t="n">
+      <c r="H71" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A72" s="7" t="n">
+      <c r="A72" s="9" t="n">
         <v>183939</v>
       </c>
-      <c r="B72" s="7" t="n">
+      <c r="B72" s="9" t="n">
         <v>216</v>
       </c>
       <c r="D72" s="1" t="n">
@@ -6302,18 +6500,18 @@
       <c r="E72" s="1" t="n">
         <v>234</v>
       </c>
-      <c r="G72" s="7" t="n">
+      <c r="G72" s="9" t="n">
         <v>183939</v>
       </c>
-      <c r="H72" s="7" t="n">
+      <c r="H72" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A73" s="7" t="n">
+      <c r="A73" s="9" t="n">
         <v>188418</v>
       </c>
-      <c r="B73" s="7" t="n">
+      <c r="B73" s="9" t="n">
         <v>212</v>
       </c>
       <c r="D73" s="1" t="n">
@@ -6322,21 +6520,21 @@
       <c r="E73" s="1" t="n">
         <v>232</v>
       </c>
-      <c r="G73" s="7" t="n">
+      <c r="G73" s="9" t="n">
         <v>188418</v>
       </c>
-      <c r="H73" s="7" t="n">
-        <v>88</v>
-      </c>
-      <c r="L73" s="0"/>
+      <c r="H73" s="9" t="n">
+        <v>88</v>
+      </c>
       <c r="M73" s="0"/>
       <c r="N73" s="0"/>
+      <c r="O73" s="0"/>
     </row>
     <row r="74" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A74" s="7" t="n">
+      <c r="A74" s="9" t="n">
         <v>192897</v>
       </c>
-      <c r="B74" s="7" t="n">
+      <c r="B74" s="9" t="n">
         <v>209</v>
       </c>
       <c r="D74" s="1" t="n">
@@ -6345,21 +6543,21 @@
       <c r="E74" s="1" t="n">
         <v>231</v>
       </c>
-      <c r="G74" s="7" t="n">
+      <c r="G74" s="9" t="n">
         <v>192897</v>
       </c>
-      <c r="H74" s="7" t="n">
-        <v>88</v>
-      </c>
-      <c r="L74" s="0"/>
+      <c r="H74" s="9" t="n">
+        <v>88</v>
+      </c>
       <c r="M74" s="0"/>
       <c r="N74" s="0"/>
+      <c r="O74" s="0"/>
     </row>
     <row r="75" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A75" s="7" t="n">
+      <c r="A75" s="9" t="n">
         <v>197376</v>
       </c>
-      <c r="B75" s="7" t="n">
+      <c r="B75" s="9" t="n">
         <v>206</v>
       </c>
       <c r="D75" s="1" t="n">
@@ -6368,21 +6566,21 @@
       <c r="E75" s="1" t="n">
         <v>229</v>
       </c>
-      <c r="G75" s="7" t="n">
+      <c r="G75" s="9" t="n">
         <v>197376</v>
       </c>
-      <c r="H75" s="7" t="n">
-        <v>88</v>
-      </c>
-      <c r="L75" s="0"/>
+      <c r="H75" s="9" t="n">
+        <v>88</v>
+      </c>
       <c r="M75" s="0"/>
       <c r="N75" s="0"/>
+      <c r="O75" s="0"/>
     </row>
     <row r="76" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A76" s="7" t="n">
+      <c r="A76" s="9" t="n">
         <v>201855</v>
       </c>
-      <c r="B76" s="7" t="n">
+      <c r="B76" s="9" t="n">
         <v>203</v>
       </c>
       <c r="D76" s="1" t="n">
@@ -6391,21 +6589,21 @@
       <c r="E76" s="1" t="n">
         <v>227</v>
       </c>
-      <c r="G76" s="7" t="n">
+      <c r="G76" s="9" t="n">
         <v>201855</v>
       </c>
-      <c r="H76" s="7" t="n">
-        <v>88</v>
-      </c>
-      <c r="L76" s="0"/>
+      <c r="H76" s="9" t="n">
+        <v>88</v>
+      </c>
       <c r="M76" s="0"/>
       <c r="N76" s="0"/>
+      <c r="O76" s="0"/>
     </row>
     <row r="77" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A77" s="7" t="n">
+      <c r="A77" s="9" t="n">
         <v>206334</v>
       </c>
-      <c r="B77" s="7" t="n">
+      <c r="B77" s="9" t="n">
         <v>200</v>
       </c>
       <c r="D77" s="1" t="n">
@@ -6414,21 +6612,21 @@
       <c r="E77" s="1" t="n">
         <v>226</v>
       </c>
-      <c r="G77" s="7" t="n">
+      <c r="G77" s="9" t="n">
         <v>206334</v>
       </c>
-      <c r="H77" s="7" t="n">
-        <v>88</v>
-      </c>
-      <c r="L77" s="0"/>
+      <c r="H77" s="9" t="n">
+        <v>88</v>
+      </c>
       <c r="M77" s="0"/>
       <c r="N77" s="0"/>
+      <c r="O77" s="0"/>
     </row>
     <row r="78" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A78" s="7" t="n">
+      <c r="A78" s="9" t="n">
         <v>210813</v>
       </c>
-      <c r="B78" s="7" t="n">
+      <c r="B78" s="9" t="n">
         <v>197</v>
       </c>
       <c r="D78" s="1" t="n">
@@ -6437,18 +6635,18 @@
       <c r="E78" s="1" t="n">
         <v>224</v>
       </c>
-      <c r="G78" s="7" t="n">
+      <c r="G78" s="9" t="n">
         <v>210813</v>
       </c>
-      <c r="H78" s="7" t="n">
+      <c r="H78" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A79" s="7" t="n">
+      <c r="A79" s="9" t="n">
         <v>215292</v>
       </c>
-      <c r="B79" s="7" t="n">
+      <c r="B79" s="9" t="n">
         <v>194</v>
       </c>
       <c r="D79" s="1" t="n">
@@ -6457,18 +6655,18 @@
       <c r="E79" s="1" t="n">
         <v>222</v>
       </c>
-      <c r="G79" s="7" t="n">
+      <c r="G79" s="9" t="n">
         <v>215292</v>
       </c>
-      <c r="H79" s="7" t="n">
+      <c r="H79" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A80" s="7" t="n">
+      <c r="A80" s="9" t="n">
         <v>219771</v>
       </c>
-      <c r="B80" s="7" t="n">
+      <c r="B80" s="9" t="n">
         <v>191</v>
       </c>
       <c r="D80" s="1" t="n">
@@ -6477,18 +6675,18 @@
       <c r="E80" s="1" t="n">
         <v>221</v>
       </c>
-      <c r="G80" s="7" t="n">
+      <c r="G80" s="9" t="n">
         <v>219771</v>
       </c>
-      <c r="H80" s="7" t="n">
+      <c r="H80" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A81" s="7" t="n">
+      <c r="A81" s="9" t="n">
         <v>224250</v>
       </c>
-      <c r="B81" s="7" t="n">
+      <c r="B81" s="9" t="n">
         <v>188</v>
       </c>
       <c r="D81" s="1" t="n">
@@ -6497,18 +6695,18 @@
       <c r="E81" s="1" t="n">
         <v>219</v>
       </c>
-      <c r="G81" s="7" t="n">
+      <c r="G81" s="9" t="n">
         <v>224250</v>
       </c>
-      <c r="H81" s="7" t="n">
+      <c r="H81" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A82" s="7" t="n">
+      <c r="A82" s="9" t="n">
         <v>228729</v>
       </c>
-      <c r="B82" s="7" t="n">
+      <c r="B82" s="9" t="n">
         <v>185</v>
       </c>
       <c r="D82" s="1" t="n">
@@ -6517,18 +6715,18 @@
       <c r="E82" s="1" t="n">
         <v>218</v>
       </c>
-      <c r="G82" s="7" t="n">
+      <c r="G82" s="9" t="n">
         <v>228729</v>
       </c>
-      <c r="H82" s="7" t="n">
+      <c r="H82" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A83" s="7" t="n">
+      <c r="A83" s="9" t="n">
         <v>233208</v>
       </c>
-      <c r="B83" s="7" t="n">
+      <c r="B83" s="9" t="n">
         <v>183</v>
       </c>
       <c r="D83" s="1" t="n">
@@ -6537,18 +6735,18 @@
       <c r="E83" s="1" t="n">
         <v>216</v>
       </c>
-      <c r="G83" s="7" t="n">
+      <c r="G83" s="9" t="n">
         <v>233208</v>
       </c>
-      <c r="H83" s="7" t="n">
+      <c r="H83" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A84" s="7" t="n">
+      <c r="A84" s="9" t="n">
         <v>237687</v>
       </c>
-      <c r="B84" s="7" t="n">
+      <c r="B84" s="9" t="n">
         <v>180</v>
       </c>
       <c r="D84" s="1" t="n">
@@ -6557,18 +6755,18 @@
       <c r="E84" s="1" t="n">
         <v>215</v>
       </c>
-      <c r="G84" s="7" t="n">
+      <c r="G84" s="9" t="n">
         <v>237687</v>
       </c>
-      <c r="H84" s="7" t="n">
+      <c r="H84" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A85" s="7" t="n">
+      <c r="A85" s="9" t="n">
         <v>242166</v>
       </c>
-      <c r="B85" s="7" t="n">
+      <c r="B85" s="9" t="n">
         <v>178</v>
       </c>
       <c r="D85" s="1" t="n">
@@ -6577,18 +6775,18 @@
       <c r="E85" s="1" t="n">
         <v>214</v>
       </c>
-      <c r="G85" s="7" t="n">
+      <c r="G85" s="9" t="n">
         <v>242166</v>
       </c>
-      <c r="H85" s="7" t="n">
+      <c r="H85" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A86" s="7" t="n">
+      <c r="A86" s="9" t="n">
         <v>246645</v>
       </c>
-      <c r="B86" s="7" t="n">
+      <c r="B86" s="9" t="n">
         <v>175</v>
       </c>
       <c r="D86" s="1" t="n">
@@ -6597,18 +6795,18 @@
       <c r="E86" s="1" t="n">
         <v>212</v>
       </c>
-      <c r="G86" s="7" t="n">
+      <c r="G86" s="9" t="n">
         <v>246645</v>
       </c>
-      <c r="H86" s="7" t="n">
+      <c r="H86" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A87" s="7" t="n">
+      <c r="A87" s="9" t="n">
         <v>251124</v>
       </c>
-      <c r="B87" s="7" t="n">
+      <c r="B87" s="9" t="n">
         <v>173</v>
       </c>
       <c r="D87" s="1" t="n">
@@ -6617,18 +6815,18 @@
       <c r="E87" s="1" t="n">
         <v>211</v>
       </c>
-      <c r="G87" s="7" t="n">
+      <c r="G87" s="9" t="n">
         <v>251124</v>
       </c>
-      <c r="H87" s="7" t="n">
+      <c r="H87" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A88" s="7" t="n">
+      <c r="A88" s="9" t="n">
         <v>255603</v>
       </c>
-      <c r="B88" s="7" t="n">
+      <c r="B88" s="9" t="n">
         <v>170</v>
       </c>
       <c r="D88" s="1" t="n">
@@ -6637,18 +6835,18 @@
       <c r="E88" s="1" t="n">
         <v>209</v>
       </c>
-      <c r="G88" s="7" t="n">
+      <c r="G88" s="9" t="n">
         <v>255603</v>
       </c>
-      <c r="H88" s="7" t="n">
+      <c r="H88" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A89" s="7" t="n">
+      <c r="A89" s="9" t="n">
         <v>260082</v>
       </c>
-      <c r="B89" s="7" t="n">
+      <c r="B89" s="9" t="n">
         <v>168</v>
       </c>
       <c r="D89" s="1" t="n">
@@ -6657,18 +6855,18 @@
       <c r="E89" s="1" t="n">
         <v>208</v>
       </c>
-      <c r="G89" s="7" t="n">
+      <c r="G89" s="9" t="n">
         <v>260082</v>
       </c>
-      <c r="H89" s="7" t="n">
+      <c r="H89" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A90" s="7" t="n">
+      <c r="A90" s="9" t="n">
         <v>264561</v>
       </c>
-      <c r="B90" s="7" t="n">
+      <c r="B90" s="9" t="n">
         <v>166</v>
       </c>
       <c r="D90" s="1" t="n">
@@ -6677,18 +6875,18 @@
       <c r="E90" s="1" t="n">
         <v>207</v>
       </c>
-      <c r="G90" s="7" t="n">
+      <c r="G90" s="9" t="n">
         <v>264561</v>
       </c>
-      <c r="H90" s="7" t="n">
+      <c r="H90" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A91" s="7" t="n">
+      <c r="A91" s="9" t="n">
         <v>269040</v>
       </c>
-      <c r="B91" s="7" t="n">
+      <c r="B91" s="9" t="n">
         <v>163</v>
       </c>
       <c r="D91" s="1" t="n">
@@ -6697,18 +6895,18 @@
       <c r="E91" s="1" t="n">
         <v>206</v>
       </c>
-      <c r="G91" s="7" t="n">
+      <c r="G91" s="9" t="n">
         <v>269040</v>
       </c>
-      <c r="H91" s="7" t="n">
+      <c r="H91" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A92" s="7" t="n">
+      <c r="A92" s="9" t="n">
         <v>273519</v>
       </c>
-      <c r="B92" s="7" t="n">
+      <c r="B92" s="9" t="n">
         <v>161</v>
       </c>
       <c r="D92" s="1" t="n">
@@ -6717,18 +6915,18 @@
       <c r="E92" s="1" t="n">
         <v>204</v>
       </c>
-      <c r="G92" s="7" t="n">
+      <c r="G92" s="9" t="n">
         <v>273519</v>
       </c>
-      <c r="H92" s="7" t="n">
+      <c r="H92" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A93" s="7" t="n">
+      <c r="A93" s="9" t="n">
         <v>277998</v>
       </c>
-      <c r="B93" s="7" t="n">
+      <c r="B93" s="9" t="n">
         <v>159</v>
       </c>
       <c r="D93" s="1" t="n">
@@ -6737,18 +6935,18 @@
       <c r="E93" s="1" t="n">
         <v>203</v>
       </c>
-      <c r="G93" s="7" t="n">
+      <c r="G93" s="9" t="n">
         <v>277998</v>
       </c>
-      <c r="H93" s="7" t="n">
+      <c r="H93" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A94" s="7" t="n">
+      <c r="A94" s="9" t="n">
         <v>282477</v>
       </c>
-      <c r="B94" s="7" t="n">
+      <c r="B94" s="9" t="n">
         <v>157</v>
       </c>
       <c r="D94" s="1" t="n">
@@ -6757,18 +6955,18 @@
       <c r="E94" s="1" t="n">
         <v>202</v>
       </c>
-      <c r="G94" s="7" t="n">
+      <c r="G94" s="9" t="n">
         <v>282477</v>
       </c>
-      <c r="H94" s="7" t="n">
+      <c r="H94" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A95" s="7" t="n">
+      <c r="A95" s="9" t="n">
         <v>286956</v>
       </c>
-      <c r="B95" s="7" t="n">
+      <c r="B95" s="9" t="n">
         <v>155</v>
       </c>
       <c r="D95" s="1" t="n">
@@ -6777,18 +6975,18 @@
       <c r="E95" s="1" t="n">
         <v>201</v>
       </c>
-      <c r="G95" s="7" t="n">
+      <c r="G95" s="9" t="n">
         <v>286956</v>
       </c>
-      <c r="H95" s="7" t="n">
+      <c r="H95" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A96" s="7" t="n">
+      <c r="A96" s="9" t="n">
         <v>291435</v>
       </c>
-      <c r="B96" s="7" t="n">
+      <c r="B96" s="9" t="n">
         <v>153</v>
       </c>
       <c r="D96" s="1" t="n">
@@ -6797,18 +6995,18 @@
       <c r="E96" s="1" t="n">
         <v>200</v>
       </c>
-      <c r="G96" s="7" t="n">
+      <c r="G96" s="9" t="n">
         <v>291435</v>
       </c>
-      <c r="H96" s="7" t="n">
+      <c r="H96" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A97" s="7" t="n">
+      <c r="A97" s="9" t="n">
         <v>295914</v>
       </c>
-      <c r="B97" s="7" t="n">
+      <c r="B97" s="9" t="n">
         <v>151</v>
       </c>
       <c r="D97" s="1" t="n">
@@ -6817,18 +7015,18 @@
       <c r="E97" s="1" t="n">
         <v>199</v>
       </c>
-      <c r="G97" s="7" t="n">
+      <c r="G97" s="9" t="n">
         <v>295914</v>
       </c>
-      <c r="H97" s="7" t="n">
+      <c r="H97" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A98" s="7" t="n">
+      <c r="A98" s="9" t="n">
         <v>300393</v>
       </c>
-      <c r="B98" s="7" t="n">
+      <c r="B98" s="9" t="n">
         <v>149</v>
       </c>
       <c r="D98" s="1" t="n">
@@ -6837,18 +7035,18 @@
       <c r="E98" s="1" t="n">
         <v>197</v>
       </c>
-      <c r="G98" s="7" t="n">
+      <c r="G98" s="9" t="n">
         <v>300393</v>
       </c>
-      <c r="H98" s="7" t="n">
+      <c r="H98" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A99" s="7" t="n">
+      <c r="A99" s="9" t="n">
         <v>304872</v>
       </c>
-      <c r="B99" s="7" t="n">
+      <c r="B99" s="9" t="n">
         <v>147</v>
       </c>
       <c r="D99" s="1" t="n">
@@ -6857,18 +7055,18 @@
       <c r="E99" s="1" t="n">
         <v>196</v>
       </c>
-      <c r="G99" s="7" t="n">
+      <c r="G99" s="9" t="n">
         <v>304872</v>
       </c>
-      <c r="H99" s="7" t="n">
+      <c r="H99" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A100" s="7" t="n">
+      <c r="A100" s="9" t="n">
         <v>309351</v>
       </c>
-      <c r="B100" s="7" t="n">
+      <c r="B100" s="9" t="n">
         <v>145</v>
       </c>
       <c r="D100" s="1" t="n">
@@ -6877,18 +7075,18 @@
       <c r="E100" s="1" t="n">
         <v>195</v>
       </c>
-      <c r="G100" s="7" t="n">
+      <c r="G100" s="9" t="n">
         <v>309351</v>
       </c>
-      <c r="H100" s="7" t="n">
+      <c r="H100" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A101" s="7" t="n">
+      <c r="A101" s="9" t="n">
         <v>313830</v>
       </c>
-      <c r="B101" s="7" t="n">
+      <c r="B101" s="9" t="n">
         <v>143</v>
       </c>
       <c r="D101" s="1" t="n">
@@ -6897,18 +7095,18 @@
       <c r="E101" s="1" t="n">
         <v>194</v>
       </c>
-      <c r="G101" s="7" t="n">
+      <c r="G101" s="9" t="n">
         <v>313830</v>
       </c>
-      <c r="H101" s="7" t="n">
+      <c r="H101" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A102" s="7" t="n">
+      <c r="A102" s="9" t="n">
         <v>318309</v>
       </c>
-      <c r="B102" s="7" t="n">
+      <c r="B102" s="9" t="n">
         <v>141</v>
       </c>
       <c r="D102" s="1" t="n">
@@ -6917,18 +7115,18 @@
       <c r="E102" s="1" t="n">
         <v>193</v>
       </c>
-      <c r="G102" s="7" t="n">
+      <c r="G102" s="9" t="n">
         <v>318309</v>
       </c>
-      <c r="H102" s="7" t="n">
+      <c r="H102" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A103" s="7" t="n">
+      <c r="A103" s="9" t="n">
         <v>322788</v>
       </c>
-      <c r="B103" s="7" t="n">
+      <c r="B103" s="9" t="n">
         <v>139</v>
       </c>
       <c r="D103" s="1" t="n">
@@ -6937,18 +7135,18 @@
       <c r="E103" s="1" t="n">
         <v>192</v>
       </c>
-      <c r="G103" s="7" t="n">
+      <c r="G103" s="9" t="n">
         <v>322788</v>
       </c>
-      <c r="H103" s="7" t="n">
+      <c r="H103" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A104" s="7" t="n">
+      <c r="A104" s="9" t="n">
         <v>327267</v>
       </c>
-      <c r="B104" s="7" t="n">
+      <c r="B104" s="9" t="n">
         <v>138</v>
       </c>
       <c r="D104" s="1" t="n">
@@ -6957,18 +7155,18 @@
       <c r="E104" s="1" t="n">
         <v>191</v>
       </c>
-      <c r="G104" s="7" t="n">
+      <c r="G104" s="9" t="n">
         <v>327267</v>
       </c>
-      <c r="H104" s="7" t="n">
+      <c r="H104" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A105" s="7" t="n">
+      <c r="A105" s="9" t="n">
         <v>331746</v>
       </c>
-      <c r="B105" s="7" t="n">
+      <c r="B105" s="9" t="n">
         <v>136</v>
       </c>
       <c r="D105" s="1" t="n">
@@ -6977,18 +7175,18 @@
       <c r="E105" s="1" t="n">
         <v>190</v>
       </c>
-      <c r="G105" s="7" t="n">
+      <c r="G105" s="9" t="n">
         <v>331746</v>
       </c>
-      <c r="H105" s="7" t="n">
+      <c r="H105" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A106" s="7" t="n">
+      <c r="A106" s="9" t="n">
         <v>336225</v>
       </c>
-      <c r="B106" s="7" t="n">
+      <c r="B106" s="9" t="n">
         <v>134</v>
       </c>
       <c r="D106" s="1" t="n">
@@ -6997,18 +7195,18 @@
       <c r="E106" s="1" t="n">
         <v>189</v>
       </c>
-      <c r="G106" s="7" t="n">
+      <c r="G106" s="9" t="n">
         <v>336225</v>
       </c>
-      <c r="H106" s="7" t="n">
+      <c r="H106" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A107" s="7" t="n">
+      <c r="A107" s="9" t="n">
         <v>340704</v>
       </c>
-      <c r="B107" s="7" t="n">
+      <c r="B107" s="9" t="n">
         <v>133</v>
       </c>
       <c r="D107" s="1" t="n">
@@ -7017,18 +7215,18 @@
       <c r="E107" s="1" t="n">
         <v>188</v>
       </c>
-      <c r="G107" s="7" t="n">
+      <c r="G107" s="9" t="n">
         <v>340704</v>
       </c>
-      <c r="H107" s="7" t="n">
+      <c r="H107" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A108" s="7" t="n">
+      <c r="A108" s="9" t="n">
         <v>345183</v>
       </c>
-      <c r="B108" s="7" t="n">
+      <c r="B108" s="9" t="n">
         <v>131</v>
       </c>
       <c r="D108" s="1" t="n">
@@ -7037,18 +7235,18 @@
       <c r="E108" s="1" t="n">
         <v>187</v>
       </c>
-      <c r="G108" s="7" t="n">
+      <c r="G108" s="9" t="n">
         <v>345183</v>
       </c>
-      <c r="H108" s="7" t="n">
+      <c r="H108" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A109" s="7" t="n">
+      <c r="A109" s="9" t="n">
         <v>349662</v>
       </c>
-      <c r="B109" s="7" t="n">
+      <c r="B109" s="9" t="n">
         <v>129</v>
       </c>
       <c r="D109" s="1" t="n">
@@ -7057,18 +7255,18 @@
       <c r="E109" s="1" t="n">
         <v>186</v>
       </c>
-      <c r="G109" s="7" t="n">
+      <c r="G109" s="9" t="n">
         <v>349662</v>
       </c>
-      <c r="H109" s="7" t="n">
+      <c r="H109" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A110" s="7" t="n">
+      <c r="A110" s="9" t="n">
         <v>354141</v>
       </c>
-      <c r="B110" s="7" t="n">
+      <c r="B110" s="9" t="n">
         <v>128</v>
       </c>
       <c r="D110" s="1" t="n">
@@ -7077,18 +7275,18 @@
       <c r="E110" s="1" t="n">
         <v>185</v>
       </c>
-      <c r="G110" s="7" t="n">
+      <c r="G110" s="9" t="n">
         <v>354141</v>
       </c>
-      <c r="H110" s="7" t="n">
+      <c r="H110" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A111" s="7" t="n">
+      <c r="A111" s="9" t="n">
         <v>358620</v>
       </c>
-      <c r="B111" s="7" t="n">
+      <c r="B111" s="9" t="n">
         <v>126</v>
       </c>
       <c r="D111" s="1" t="n">
@@ -7097,18 +7295,18 @@
       <c r="E111" s="1" t="n">
         <v>185</v>
       </c>
-      <c r="G111" s="7" t="n">
+      <c r="G111" s="9" t="n">
         <v>358620</v>
       </c>
-      <c r="H111" s="7" t="n">
+      <c r="H111" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A112" s="7" t="n">
+      <c r="A112" s="9" t="n">
         <v>363099</v>
       </c>
-      <c r="B112" s="7" t="n">
+      <c r="B112" s="9" t="n">
         <v>125</v>
       </c>
       <c r="D112" s="1" t="n">
@@ -7117,18 +7315,18 @@
       <c r="E112" s="1" t="n">
         <v>184</v>
       </c>
-      <c r="G112" s="7" t="n">
+      <c r="G112" s="9" t="n">
         <v>363099</v>
       </c>
-      <c r="H112" s="7" t="n">
+      <c r="H112" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A113" s="7" t="n">
+      <c r="A113" s="9" t="n">
         <v>367578</v>
       </c>
-      <c r="B113" s="7" t="n">
+      <c r="B113" s="9" t="n">
         <v>123</v>
       </c>
       <c r="D113" s="1" t="n">
@@ -7137,18 +7335,18 @@
       <c r="E113" s="1" t="n">
         <v>183</v>
       </c>
-      <c r="G113" s="7" t="n">
+      <c r="G113" s="9" t="n">
         <v>367578</v>
       </c>
-      <c r="H113" s="7" t="n">
+      <c r="H113" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A114" s="7" t="n">
+      <c r="A114" s="9" t="n">
         <v>372057</v>
       </c>
-      <c r="B114" s="7" t="n">
+      <c r="B114" s="9" t="n">
         <v>122</v>
       </c>
       <c r="D114" s="1" t="n">
@@ -7157,18 +7355,18 @@
       <c r="E114" s="1" t="n">
         <v>182</v>
       </c>
-      <c r="G114" s="7" t="n">
+      <c r="G114" s="9" t="n">
         <v>372057</v>
       </c>
-      <c r="H114" s="7" t="n">
+      <c r="H114" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A115" s="7" t="n">
+      <c r="A115" s="9" t="n">
         <v>376536</v>
       </c>
-      <c r="B115" s="7" t="n">
+      <c r="B115" s="9" t="n">
         <v>120</v>
       </c>
       <c r="D115" s="1" t="n">
@@ -7177,18 +7375,18 @@
       <c r="E115" s="1" t="n">
         <v>181</v>
       </c>
-      <c r="G115" s="7" t="n">
+      <c r="G115" s="9" t="n">
         <v>376536</v>
       </c>
-      <c r="H115" s="7" t="n">
+      <c r="H115" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A116" s="7" t="n">
+      <c r="A116" s="9" t="n">
         <v>381015</v>
       </c>
-      <c r="B116" s="7" t="n">
+      <c r="B116" s="9" t="n">
         <v>119</v>
       </c>
       <c r="D116" s="1" t="n">
@@ -7197,18 +7395,18 @@
       <c r="E116" s="1" t="n">
         <v>180</v>
       </c>
-      <c r="G116" s="7" t="n">
+      <c r="G116" s="9" t="n">
         <v>381015</v>
       </c>
-      <c r="H116" s="7" t="n">
+      <c r="H116" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A117" s="7" t="n">
+      <c r="A117" s="9" t="n">
         <v>385494</v>
       </c>
-      <c r="B117" s="7" t="n">
+      <c r="B117" s="9" t="n">
         <v>147</v>
       </c>
       <c r="D117" s="1" t="n">
@@ -7217,18 +7415,18 @@
       <c r="E117" s="1" t="n">
         <v>179</v>
       </c>
-      <c r="G117" s="7" t="n">
+      <c r="G117" s="9" t="n">
         <v>385494</v>
       </c>
-      <c r="H117" s="7" t="n">
+      <c r="H117" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A118" s="7" t="n">
+      <c r="A118" s="9" t="n">
         <v>389973</v>
       </c>
-      <c r="B118" s="7" t="n">
+      <c r="B118" s="9" t="n">
         <v>224</v>
       </c>
       <c r="D118" s="1" t="n">
@@ -7237,18 +7435,18 @@
       <c r="E118" s="1" t="n">
         <v>179</v>
       </c>
-      <c r="G118" s="7" t="n">
+      <c r="G118" s="9" t="n">
         <v>389973</v>
       </c>
-      <c r="H118" s="7" t="n">
+      <c r="H118" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="7" t="n">
+      <c r="A119" s="9" t="n">
         <v>394452</v>
       </c>
-      <c r="B119" s="7" t="n">
+      <c r="B119" s="9" t="n">
         <v>223</v>
       </c>
       <c r="D119" s="1" t="n">
@@ -7257,18 +7455,18 @@
       <c r="E119" s="1" t="n">
         <v>178</v>
       </c>
-      <c r="G119" s="7" t="n">
+      <c r="G119" s="9" t="n">
         <v>394452</v>
       </c>
-      <c r="H119" s="7" t="n">
+      <c r="H119" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="7" t="n">
+      <c r="A120" s="9" t="n">
         <v>398931</v>
       </c>
-      <c r="B120" s="7" t="n">
+      <c r="B120" s="9" t="n">
         <v>222</v>
       </c>
       <c r="D120" s="1" t="n">
@@ -7277,18 +7475,18 @@
       <c r="E120" s="1" t="n">
         <v>177</v>
       </c>
-      <c r="G120" s="7" t="n">
+      <c r="G120" s="9" t="n">
         <v>398931</v>
       </c>
-      <c r="H120" s="7" t="n">
+      <c r="H120" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="7" t="n">
+      <c r="A121" s="9" t="n">
         <v>403410</v>
       </c>
-      <c r="B121" s="7" t="n">
+      <c r="B121" s="9" t="n">
         <v>221</v>
       </c>
       <c r="D121" s="1" t="n">
@@ -7297,18 +7495,18 @@
       <c r="E121" s="1" t="n">
         <v>176</v>
       </c>
-      <c r="G121" s="7" t="n">
+      <c r="G121" s="9" t="n">
         <v>403410</v>
       </c>
-      <c r="H121" s="7" t="n">
+      <c r="H121" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="7" t="n">
+      <c r="A122" s="9" t="n">
         <v>407889</v>
       </c>
-      <c r="B122" s="7" t="n">
+      <c r="B122" s="9" t="n">
         <v>219</v>
       </c>
       <c r="D122" s="1" t="n">
@@ -7317,18 +7515,18 @@
       <c r="E122" s="1" t="n">
         <v>175</v>
       </c>
-      <c r="G122" s="7" t="n">
+      <c r="G122" s="9" t="n">
         <v>407889</v>
       </c>
-      <c r="H122" s="7" t="n">
+      <c r="H122" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="7" t="n">
+      <c r="A123" s="9" t="n">
         <v>412368</v>
       </c>
-      <c r="B123" s="7" t="n">
+      <c r="B123" s="9" t="n">
         <v>218</v>
       </c>
       <c r="D123" s="1" t="n">
@@ -7337,18 +7535,18 @@
       <c r="E123" s="1" t="n">
         <v>175</v>
       </c>
-      <c r="G123" s="7" t="n">
+      <c r="G123" s="9" t="n">
         <v>412368</v>
       </c>
-      <c r="H123" s="7" t="n">
+      <c r="H123" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="7" t="n">
+      <c r="A124" s="9" t="n">
         <v>416847</v>
       </c>
-      <c r="B124" s="7" t="n">
+      <c r="B124" s="9" t="n">
         <v>217</v>
       </c>
       <c r="D124" s="1" t="n">
@@ -7357,18 +7555,18 @@
       <c r="E124" s="1" t="n">
         <v>174</v>
       </c>
-      <c r="G124" s="7" t="n">
+      <c r="G124" s="9" t="n">
         <v>416847</v>
       </c>
-      <c r="H124" s="7" t="n">
+      <c r="H124" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="7" t="n">
+      <c r="A125" s="9" t="n">
         <v>421326</v>
       </c>
-      <c r="B125" s="7" t="n">
+      <c r="B125" s="9" t="n">
         <v>216</v>
       </c>
       <c r="D125" s="1" t="n">
@@ -7377,18 +7575,18 @@
       <c r="E125" s="1" t="n">
         <v>173</v>
       </c>
-      <c r="G125" s="7" t="n">
+      <c r="G125" s="9" t="n">
         <v>421326</v>
       </c>
-      <c r="H125" s="7" t="n">
+      <c r="H125" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="7" t="n">
+      <c r="A126" s="9" t="n">
         <v>425805</v>
       </c>
-      <c r="B126" s="7" t="n">
+      <c r="B126" s="9" t="n">
         <v>214</v>
       </c>
       <c r="D126" s="1" t="n">
@@ -7397,18 +7595,18 @@
       <c r="E126" s="1" t="n">
         <v>172</v>
       </c>
-      <c r="G126" s="7" t="n">
+      <c r="G126" s="9" t="n">
         <v>425805</v>
       </c>
-      <c r="H126" s="7" t="n">
+      <c r="H126" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="7" t="n">
+      <c r="A127" s="9" t="n">
         <v>430284</v>
       </c>
-      <c r="B127" s="7" t="n">
+      <c r="B127" s="9" t="n">
         <v>213</v>
       </c>
       <c r="D127" s="1" t="n">
@@ -7417,18 +7615,18 @@
       <c r="E127" s="1" t="n">
         <v>172</v>
       </c>
-      <c r="G127" s="7" t="n">
+      <c r="G127" s="9" t="n">
         <v>430284</v>
       </c>
-      <c r="H127" s="7" t="n">
+      <c r="H127" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="7" t="n">
+      <c r="A128" s="9" t="n">
         <v>434763</v>
       </c>
-      <c r="B128" s="7" t="n">
+      <c r="B128" s="9" t="n">
         <v>212</v>
       </c>
       <c r="D128" s="1" t="n">
@@ -7437,18 +7635,18 @@
       <c r="E128" s="1" t="n">
         <v>171</v>
       </c>
-      <c r="G128" s="7" t="n">
+      <c r="G128" s="9" t="n">
         <v>434763</v>
       </c>
-      <c r="H128" s="7" t="n">
+      <c r="H128" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="129" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="7" t="n">
+      <c r="A129" s="9" t="n">
         <v>439242</v>
       </c>
-      <c r="B129" s="7" t="n">
+      <c r="B129" s="9" t="n">
         <v>211</v>
       </c>
       <c r="D129" s="1" t="n">
@@ -7457,18 +7655,18 @@
       <c r="E129" s="1" t="n">
         <v>170</v>
       </c>
-      <c r="G129" s="7" t="n">
+      <c r="G129" s="9" t="n">
         <v>439242</v>
       </c>
-      <c r="H129" s="7" t="n">
+      <c r="H129" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="130" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="7" t="n">
+      <c r="A130" s="9" t="n">
         <v>443721</v>
       </c>
-      <c r="B130" s="7" t="n">
+      <c r="B130" s="9" t="n">
         <v>210</v>
       </c>
       <c r="D130" s="1" t="n">
@@ -7477,18 +7675,18 @@
       <c r="E130" s="1" t="n">
         <v>169</v>
       </c>
-      <c r="G130" s="7" t="n">
+      <c r="G130" s="9" t="n">
         <v>443721</v>
       </c>
-      <c r="H130" s="7" t="n">
+      <c r="H130" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="131" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="7" t="n">
+      <c r="A131" s="9" t="n">
         <v>448200</v>
       </c>
-      <c r="B131" s="7" t="n">
+      <c r="B131" s="9" t="n">
         <v>208</v>
       </c>
       <c r="D131" s="1" t="n">
@@ -7497,18 +7695,18 @@
       <c r="E131" s="1" t="n">
         <v>169</v>
       </c>
-      <c r="G131" s="7" t="n">
+      <c r="G131" s="9" t="n">
         <v>448200</v>
       </c>
-      <c r="H131" s="7" t="n">
+      <c r="H131" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="132" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="7" t="n">
+      <c r="A132" s="9" t="n">
         <v>452679</v>
       </c>
-      <c r="B132" s="7" t="n">
+      <c r="B132" s="9" t="n">
         <v>207</v>
       </c>
       <c r="D132" s="1" t="n">
@@ -7517,18 +7715,18 @@
       <c r="E132" s="1" t="n">
         <v>168</v>
       </c>
-      <c r="G132" s="7" t="n">
+      <c r="G132" s="9" t="n">
         <v>452679</v>
       </c>
-      <c r="H132" s="7" t="n">
+      <c r="H132" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="133" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="7" t="n">
+      <c r="A133" s="9" t="n">
         <v>457158</v>
       </c>
-      <c r="B133" s="7" t="n">
+      <c r="B133" s="9" t="n">
         <v>206</v>
       </c>
       <c r="D133" s="1" t="n">
@@ -7537,18 +7735,18 @@
       <c r="E133" s="1" t="n">
         <v>167</v>
       </c>
-      <c r="G133" s="7" t="n">
+      <c r="G133" s="9" t="n">
         <v>457158</v>
       </c>
-      <c r="H133" s="7" t="n">
+      <c r="H133" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="134" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="7" t="n">
+      <c r="A134" s="9" t="n">
         <v>461637</v>
       </c>
-      <c r="B134" s="7" t="n">
+      <c r="B134" s="9" t="n">
         <v>205</v>
       </c>
       <c r="D134" s="1" t="n">
@@ -7557,18 +7755,18 @@
       <c r="E134" s="1" t="n">
         <v>167</v>
       </c>
-      <c r="G134" s="7" t="n">
+      <c r="G134" s="9" t="n">
         <v>461637</v>
       </c>
-      <c r="H134" s="7" t="n">
+      <c r="H134" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="135" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A135" s="7" t="n">
+      <c r="A135" s="9" t="n">
         <v>466116</v>
       </c>
-      <c r="B135" s="7" t="n">
+      <c r="B135" s="9" t="n">
         <v>204</v>
       </c>
       <c r="D135" s="1" t="n">
@@ -7577,18 +7775,18 @@
       <c r="E135" s="1" t="n">
         <v>166</v>
       </c>
-      <c r="G135" s="7" t="n">
+      <c r="G135" s="9" t="n">
         <v>466116</v>
       </c>
-      <c r="H135" s="7" t="n">
+      <c r="H135" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="136" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A136" s="7" t="n">
+      <c r="A136" s="9" t="n">
         <v>470595</v>
       </c>
-      <c r="B136" s="7" t="n">
+      <c r="B136" s="9" t="n">
         <v>203</v>
       </c>
       <c r="D136" s="1" t="n">
@@ -7597,18 +7795,18 @@
       <c r="E136" s="1" t="n">
         <v>165</v>
       </c>
-      <c r="G136" s="7" t="n">
+      <c r="G136" s="9" t="n">
         <v>470595</v>
       </c>
-      <c r="H136" s="7" t="n">
+      <c r="H136" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="137" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="7" t="n">
+      <c r="A137" s="9" t="n">
         <v>475074</v>
       </c>
-      <c r="B137" s="7" t="n">
+      <c r="B137" s="9" t="n">
         <v>202</v>
       </c>
       <c r="D137" s="1" t="n">
@@ -7617,18 +7815,18 @@
       <c r="E137" s="1" t="n">
         <v>165</v>
       </c>
-      <c r="G137" s="7" t="n">
+      <c r="G137" s="9" t="n">
         <v>475074</v>
       </c>
-      <c r="H137" s="7" t="n">
+      <c r="H137" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="138" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A138" s="7" t="n">
+      <c r="A138" s="9" t="n">
         <v>479553</v>
       </c>
-      <c r="B138" s="7" t="n">
+      <c r="B138" s="9" t="n">
         <v>201</v>
       </c>
       <c r="D138" s="1" t="n">
@@ -7637,18 +7835,18 @@
       <c r="E138" s="1" t="n">
         <v>164</v>
       </c>
-      <c r="G138" s="7" t="n">
+      <c r="G138" s="9" t="n">
         <v>479553</v>
       </c>
-      <c r="H138" s="7" t="n">
+      <c r="H138" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="139" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A139" s="7" t="n">
+      <c r="A139" s="9" t="n">
         <v>484032</v>
       </c>
-      <c r="B139" s="7" t="n">
+      <c r="B139" s="9" t="n">
         <v>199</v>
       </c>
       <c r="D139" s="1" t="n">
@@ -7657,18 +7855,18 @@
       <c r="E139" s="1" t="n">
         <v>163</v>
       </c>
-      <c r="G139" s="7" t="n">
+      <c r="G139" s="9" t="n">
         <v>484032</v>
       </c>
-      <c r="H139" s="7" t="n">
+      <c r="H139" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="140" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A140" s="7" t="n">
+      <c r="A140" s="9" t="n">
         <v>488511</v>
       </c>
-      <c r="B140" s="7" t="n">
+      <c r="B140" s="9" t="n">
         <v>198</v>
       </c>
       <c r="D140" s="1" t="n">
@@ -7677,18 +7875,18 @@
       <c r="E140" s="1" t="n">
         <v>163</v>
       </c>
-      <c r="G140" s="7" t="n">
+      <c r="G140" s="9" t="n">
         <v>488511</v>
       </c>
-      <c r="H140" s="7" t="n">
+      <c r="H140" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A141" s="7" t="n">
+      <c r="A141" s="9" t="n">
         <v>492990</v>
       </c>
-      <c r="B141" s="7" t="n">
+      <c r="B141" s="9" t="n">
         <v>197</v>
       </c>
       <c r="D141" s="1" t="n">
@@ -7697,18 +7895,18 @@
       <c r="E141" s="1" t="n">
         <v>162</v>
       </c>
-      <c r="G141" s="7" t="n">
+      <c r="G141" s="9" t="n">
         <v>492990</v>
       </c>
-      <c r="H141" s="7" t="n">
+      <c r="H141" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A142" s="7" t="n">
+      <c r="A142" s="9" t="n">
         <v>497469</v>
       </c>
-      <c r="B142" s="7" t="n">
+      <c r="B142" s="9" t="n">
         <v>196</v>
       </c>
       <c r="D142" s="1" t="n">
@@ -7717,18 +7915,18 @@
       <c r="E142" s="1" t="n">
         <v>162</v>
       </c>
-      <c r="G142" s="7" t="n">
+      <c r="G142" s="9" t="n">
         <v>497469</v>
       </c>
-      <c r="H142" s="7" t="n">
+      <c r="H142" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="7" t="n">
+      <c r="A143" s="9" t="n">
         <v>501948</v>
       </c>
-      <c r="B143" s="7" t="n">
+      <c r="B143" s="9" t="n">
         <v>195</v>
       </c>
       <c r="D143" s="1" t="n">
@@ -7737,18 +7935,18 @@
       <c r="E143" s="1" t="n">
         <v>161</v>
       </c>
-      <c r="G143" s="7" t="n">
+      <c r="G143" s="9" t="n">
         <v>501948</v>
       </c>
-      <c r="H143" s="7" t="n">
+      <c r="H143" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A144" s="7" t="n">
+      <c r="A144" s="9" t="n">
         <v>506427</v>
       </c>
-      <c r="B144" s="7" t="n">
+      <c r="B144" s="9" t="n">
         <v>194</v>
       </c>
       <c r="D144" s="1" t="n">
@@ -7757,18 +7955,18 @@
       <c r="E144" s="1" t="n">
         <v>160</v>
       </c>
-      <c r="G144" s="7" t="n">
+      <c r="G144" s="9" t="n">
         <v>506427</v>
       </c>
-      <c r="H144" s="7" t="n">
+      <c r="H144" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A145" s="7" t="n">
+      <c r="A145" s="9" t="n">
         <v>510906</v>
       </c>
-      <c r="B145" s="7" t="n">
+      <c r="B145" s="9" t="n">
         <v>193</v>
       </c>
       <c r="D145" s="1" t="n">
@@ -7777,18 +7975,18 @@
       <c r="E145" s="1" t="n">
         <v>160</v>
       </c>
-      <c r="G145" s="7" t="n">
+      <c r="G145" s="9" t="n">
         <v>510906</v>
       </c>
-      <c r="H145" s="7" t="n">
+      <c r="H145" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="7" t="n">
+      <c r="A146" s="9" t="n">
         <v>515385</v>
       </c>
-      <c r="B146" s="7" t="n">
+      <c r="B146" s="9" t="n">
         <v>192</v>
       </c>
       <c r="D146" s="1" t="n">
@@ -7797,18 +7995,18 @@
       <c r="E146" s="1" t="n">
         <v>159</v>
       </c>
-      <c r="G146" s="7" t="n">
+      <c r="G146" s="9" t="n">
         <v>515385</v>
       </c>
-      <c r="H146" s="7" t="n">
+      <c r="H146" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="7" t="n">
+      <c r="A147" s="9" t="n">
         <v>519864</v>
       </c>
-      <c r="B147" s="7" t="n">
+      <c r="B147" s="9" t="n">
         <v>191</v>
       </c>
       <c r="D147" s="1" t="n">
@@ -7817,18 +8015,18 @@
       <c r="E147" s="1" t="n">
         <v>159</v>
       </c>
-      <c r="G147" s="7" t="n">
+      <c r="G147" s="9" t="n">
         <v>519864</v>
       </c>
-      <c r="H147" s="7" t="n">
+      <c r="H147" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="148" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A148" s="7" t="n">
+      <c r="A148" s="9" t="n">
         <v>524343</v>
       </c>
-      <c r="B148" s="7" t="n">
+      <c r="B148" s="9" t="n">
         <v>190</v>
       </c>
       <c r="D148" s="1" t="n">
@@ -7837,18 +8035,18 @@
       <c r="E148" s="1" t="n">
         <v>158</v>
       </c>
-      <c r="G148" s="7" t="n">
+      <c r="G148" s="9" t="n">
         <v>524343</v>
       </c>
-      <c r="H148" s="7" t="n">
+      <c r="H148" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A149" s="7" t="n">
+      <c r="A149" s="9" t="n">
         <v>528822</v>
       </c>
-      <c r="B149" s="7" t="n">
+      <c r="B149" s="9" t="n">
         <v>189</v>
       </c>
       <c r="D149" s="1" t="n">
@@ -7857,18 +8055,18 @@
       <c r="E149" s="1" t="n">
         <v>158</v>
       </c>
-      <c r="G149" s="7" t="n">
+      <c r="G149" s="9" t="n">
         <v>528822</v>
       </c>
-      <c r="H149" s="7" t="n">
+      <c r="H149" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A150" s="7" t="n">
+      <c r="A150" s="9" t="n">
         <v>533301</v>
       </c>
-      <c r="B150" s="7" t="n">
+      <c r="B150" s="9" t="n">
         <v>188</v>
       </c>
       <c r="D150" s="1" t="n">
@@ -7877,18 +8075,18 @@
       <c r="E150" s="1" t="n">
         <v>157</v>
       </c>
-      <c r="G150" s="7" t="n">
+      <c r="G150" s="9" t="n">
         <v>533301</v>
       </c>
-      <c r="H150" s="7" t="n">
+      <c r="H150" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A151" s="7" t="n">
+      <c r="A151" s="9" t="n">
         <v>537780</v>
       </c>
-      <c r="B151" s="7" t="n">
+      <c r="B151" s="9" t="n">
         <v>187</v>
       </c>
       <c r="D151" s="1" t="n">
@@ -7897,18 +8095,18 @@
       <c r="E151" s="1" t="n">
         <v>156</v>
       </c>
-      <c r="G151" s="7" t="n">
+      <c r="G151" s="9" t="n">
         <v>537780</v>
       </c>
-      <c r="H151" s="7" t="n">
+      <c r="H151" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A152" s="7" t="n">
+      <c r="A152" s="9" t="n">
         <v>542259</v>
       </c>
-      <c r="B152" s="7" t="n">
+      <c r="B152" s="9" t="n">
         <v>186</v>
       </c>
       <c r="D152" s="1" t="n">
@@ -7917,18 +8115,18 @@
       <c r="E152" s="1" t="n">
         <v>156</v>
       </c>
-      <c r="G152" s="7" t="n">
+      <c r="G152" s="9" t="n">
         <v>542259</v>
       </c>
-      <c r="H152" s="7" t="n">
+      <c r="H152" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A153" s="7" t="n">
+      <c r="A153" s="9" t="n">
         <v>546738</v>
       </c>
-      <c r="B153" s="7" t="n">
+      <c r="B153" s="9" t="n">
         <v>185</v>
       </c>
       <c r="D153" s="1" t="n">
@@ -7937,18 +8135,18 @@
       <c r="E153" s="1" t="n">
         <v>155</v>
       </c>
-      <c r="G153" s="7" t="n">
+      <c r="G153" s="9" t="n">
         <v>546738</v>
       </c>
-      <c r="H153" s="7" t="n">
+      <c r="H153" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A154" s="7" t="n">
+      <c r="A154" s="9" t="n">
         <v>551217</v>
       </c>
-      <c r="B154" s="7" t="n">
+      <c r="B154" s="9" t="n">
         <v>184</v>
       </c>
       <c r="D154" s="1" t="n">
@@ -7957,18 +8155,18 @@
       <c r="E154" s="1" t="n">
         <v>155</v>
       </c>
-      <c r="G154" s="7" t="n">
+      <c r="G154" s="9" t="n">
         <v>551217</v>
       </c>
-      <c r="H154" s="7" t="n">
+      <c r="H154" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A155" s="7" t="n">
+      <c r="A155" s="9" t="n">
         <v>555696</v>
       </c>
-      <c r="B155" s="7" t="n">
+      <c r="B155" s="9" t="n">
         <v>183</v>
       </c>
       <c r="D155" s="1" t="n">
@@ -7977,18 +8175,18 @@
       <c r="E155" s="1" t="n">
         <v>154</v>
       </c>
-      <c r="G155" s="7" t="n">
+      <c r="G155" s="9" t="n">
         <v>555696</v>
       </c>
-      <c r="H155" s="7" t="n">
+      <c r="H155" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A156" s="7" t="n">
+      <c r="A156" s="9" t="n">
         <v>560175</v>
       </c>
-      <c r="B156" s="7" t="n">
+      <c r="B156" s="9" t="n">
         <v>182</v>
       </c>
       <c r="D156" s="1" t="n">
@@ -7997,18 +8195,18 @@
       <c r="E156" s="1" t="n">
         <v>154</v>
       </c>
-      <c r="G156" s="7" t="n">
+      <c r="G156" s="9" t="n">
         <v>560175</v>
       </c>
-      <c r="H156" s="7" t="n">
+      <c r="H156" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A157" s="7" t="n">
+      <c r="A157" s="9" t="n">
         <v>564654</v>
       </c>
-      <c r="B157" s="7" t="n">
+      <c r="B157" s="9" t="n">
         <v>181</v>
       </c>
       <c r="D157" s="1" t="n">
@@ -8017,18 +8215,18 @@
       <c r="E157" s="1" t="n">
         <v>153</v>
       </c>
-      <c r="G157" s="7" t="n">
+      <c r="G157" s="9" t="n">
         <v>564654</v>
       </c>
-      <c r="H157" s="7" t="n">
+      <c r="H157" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A158" s="7" t="n">
+      <c r="A158" s="9" t="n">
         <v>569133</v>
       </c>
-      <c r="B158" s="7" t="n">
+      <c r="B158" s="9" t="n">
         <v>180</v>
       </c>
       <c r="D158" s="1" t="n">
@@ -8037,18 +8235,18 @@
       <c r="E158" s="1" t="n">
         <v>153</v>
       </c>
-      <c r="G158" s="7" t="n">
+      <c r="G158" s="9" t="n">
         <v>569133</v>
       </c>
-      <c r="H158" s="7" t="n">
+      <c r="H158" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A159" s="7" t="n">
+      <c r="A159" s="9" t="n">
         <v>573612</v>
       </c>
-      <c r="B159" s="7" t="n">
+      <c r="B159" s="9" t="n">
         <v>179</v>
       </c>
       <c r="D159" s="1" t="n">
@@ -8057,18 +8255,18 @@
       <c r="E159" s="1" t="n">
         <v>152</v>
       </c>
-      <c r="G159" s="7" t="n">
+      <c r="G159" s="9" t="n">
         <v>573612</v>
       </c>
-      <c r="H159" s="7" t="n">
+      <c r="H159" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A160" s="7" t="n">
+      <c r="A160" s="9" t="n">
         <v>578091</v>
       </c>
-      <c r="B160" s="7" t="n">
+      <c r="B160" s="9" t="n">
         <v>178</v>
       </c>
       <c r="D160" s="1" t="n">
@@ -8077,18 +8275,18 @@
       <c r="E160" s="1" t="n">
         <v>152</v>
       </c>
-      <c r="G160" s="7" t="n">
+      <c r="G160" s="9" t="n">
         <v>578091</v>
       </c>
-      <c r="H160" s="7" t="n">
+      <c r="H160" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A161" s="7" t="n">
+      <c r="A161" s="9" t="n">
         <v>582570</v>
       </c>
-      <c r="B161" s="7" t="n">
+      <c r="B161" s="9" t="n">
         <v>177</v>
       </c>
       <c r="D161" s="1" t="n">
@@ -8097,18 +8295,18 @@
       <c r="E161" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="G161" s="7" t="n">
+      <c r="G161" s="9" t="n">
         <v>582570</v>
       </c>
-      <c r="H161" s="7" t="n">
+      <c r="H161" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="162" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A162" s="7" t="n">
+      <c r="A162" s="9" t="n">
         <v>587049</v>
       </c>
-      <c r="B162" s="7" t="n">
+      <c r="B162" s="9" t="n">
         <v>177</v>
       </c>
       <c r="D162" s="1" t="n">
@@ -8117,18 +8315,18 @@
       <c r="E162" s="1" t="n">
         <v>151</v>
       </c>
-      <c r="G162" s="7" t="n">
+      <c r="G162" s="9" t="n">
         <v>587049</v>
       </c>
-      <c r="H162" s="7" t="n">
+      <c r="H162" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A163" s="7" t="n">
+      <c r="A163" s="9" t="n">
         <v>591528</v>
       </c>
-      <c r="B163" s="7" t="n">
+      <c r="B163" s="9" t="n">
         <v>176</v>
       </c>
       <c r="D163" s="1" t="n">
@@ -8137,18 +8335,18 @@
       <c r="E163" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="G163" s="7" t="n">
+      <c r="G163" s="9" t="n">
         <v>591528</v>
       </c>
-      <c r="H163" s="7" t="n">
+      <c r="H163" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A164" s="7" t="n">
+      <c r="A164" s="9" t="n">
         <v>596007</v>
       </c>
-      <c r="B164" s="7" t="n">
+      <c r="B164" s="9" t="n">
         <v>175</v>
       </c>
       <c r="D164" s="1" t="n">
@@ -8157,18 +8355,18 @@
       <c r="E164" s="1" t="n">
         <v>150</v>
       </c>
-      <c r="G164" s="7" t="n">
+      <c r="G164" s="9" t="n">
         <v>596007</v>
       </c>
-      <c r="H164" s="7" t="n">
+      <c r="H164" s="9" t="n">
         <v>88</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A165" s="7" t="n">
+      <c r="A165" s="9" t="n">
         <v>600486</v>
       </c>
-      <c r="B165" s="7" t="n">
+      <c r="B165" s="9" t="n">
         <v>174</v>
       </c>
       <c r="D165" s="1" t="n">
@@ -8177,10 +8375,10 @@
       <c r="E165" s="1" t="n">
         <v>149</v>
       </c>
-      <c r="G165" s="7" t="n">
+      <c r="G165" s="9" t="n">
         <v>600486</v>
       </c>
-      <c r="H165" s="7" t="n">
+      <c r="H165" s="9" t="n">
         <v>88</v>
       </c>
     </row>
@@ -9022,11 +9220,11 @@
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="A1:H1"/>
-    <mergeCell ref="J1:Q1"/>
-    <mergeCell ref="J2:Q2"/>
-    <mergeCell ref="J3:Q3"/>
-    <mergeCell ref="J4:Q4"/>
-    <mergeCell ref="J5:Q5"/>
+    <mergeCell ref="K1:R1"/>
+    <mergeCell ref="K2:R2"/>
+    <mergeCell ref="K3:R3"/>
+    <mergeCell ref="K4:R4"/>
+    <mergeCell ref="K5:R5"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0" footer="0"/>

</xml_diff>